<commit_message>
Update Ann Arbor bike counter data.
</commit_message>
<xml_diff>
--- a/data/export_data_domain_7992.xlsx
+++ b/data/export_data_domain_7992.xlsx
@@ -30491,197 +30491,4369 @@
       <c r="A2761" s="6" t="n">
         <v>44826.708333333336</v>
       </c>
-      <c r="B2761" s="1"/>
-      <c r="C2761" s="1"/>
+      <c r="B2761" s="1" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C2761" s="1" t="n">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="2762">
       <c r="A2762" s="6" t="n">
         <v>44826.71875</v>
       </c>
-      <c r="B2762" s="1"/>
-      <c r="C2762" s="1"/>
+      <c r="B2762" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C2762" s="1" t="n">
+        <v>5.0</v>
+      </c>
     </row>
     <row r="2763">
       <c r="A2763" s="6" t="n">
         <v>44826.729166666664</v>
       </c>
-      <c r="B2763" s="1"/>
-      <c r="C2763" s="1"/>
+      <c r="B2763" s="1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C2763" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="2764">
       <c r="A2764" s="6" t="n">
         <v>44826.739583333336</v>
       </c>
-      <c r="B2764" s="1"/>
-      <c r="C2764" s="1"/>
+      <c r="B2764" s="1" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C2764" s="1" t="n">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="2765">
       <c r="A2765" s="6" t="n">
         <v>44826.75</v>
       </c>
-      <c r="B2765" s="1"/>
-      <c r="C2765" s="1"/>
+      <c r="B2765" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C2765" s="1" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="2766">
       <c r="A2766" s="6" t="n">
         <v>44826.760416666664</v>
       </c>
-      <c r="B2766" s="1"/>
-      <c r="C2766" s="1"/>
+      <c r="B2766" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2766" s="1" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="2767">
       <c r="A2767" s="6" t="n">
         <v>44826.770833333336</v>
       </c>
-      <c r="B2767" s="1"/>
-      <c r="C2767" s="1"/>
+      <c r="B2767" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C2767" s="1" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="2768">
       <c r="A2768" s="6" t="n">
         <v>44826.78125</v>
       </c>
-      <c r="B2768" s="1"/>
-      <c r="C2768" s="1"/>
+      <c r="B2768" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2768" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="2769">
       <c r="A2769" s="6" t="n">
         <v>44826.791666666664</v>
       </c>
-      <c r="B2769" s="1"/>
-      <c r="C2769" s="1"/>
+      <c r="B2769" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C2769" s="1" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="2770">
       <c r="A2770" s="6" t="n">
         <v>44826.802083333336</v>
       </c>
-      <c r="B2770" s="1"/>
-      <c r="C2770" s="1"/>
+      <c r="B2770" s="1" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C2770" s="1" t="n">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="2771">
       <c r="A2771" s="6" t="n">
         <v>44826.8125</v>
       </c>
-      <c r="B2771" s="1"/>
-      <c r="C2771" s="1"/>
+      <c r="B2771" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2771" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="2772">
       <c r="A2772" s="6" t="n">
         <v>44826.822916666664</v>
       </c>
-      <c r="B2772" s="1"/>
-      <c r="C2772" s="1"/>
+      <c r="B2772" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2772" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="2773">
       <c r="A2773" s="6" t="n">
         <v>44826.833333333336</v>
       </c>
-      <c r="B2773" s="1"/>
-      <c r="C2773" s="1"/>
+      <c r="B2773" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2773" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="2774">
       <c r="A2774" s="6" t="n">
         <v>44826.84375</v>
       </c>
-      <c r="B2774" s="1"/>
-      <c r="C2774" s="1"/>
+      <c r="B2774" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C2774" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="2775">
       <c r="A2775" s="6" t="n">
         <v>44826.854166666664</v>
       </c>
-      <c r="B2775" s="1"/>
-      <c r="C2775" s="1"/>
+      <c r="B2775" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2775" s="1" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="2776">
       <c r="A2776" s="6" t="n">
         <v>44826.864583333336</v>
       </c>
-      <c r="B2776" s="1"/>
-      <c r="C2776" s="1"/>
+      <c r="B2776" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2776" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="2777">
       <c r="A2777" s="6" t="n">
         <v>44826.875</v>
       </c>
-      <c r="B2777" s="1"/>
-      <c r="C2777" s="1"/>
+      <c r="B2777" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C2777" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="2778">
       <c r="A2778" s="6" t="n">
         <v>44826.885416666664</v>
       </c>
-      <c r="B2778" s="1"/>
-      <c r="C2778" s="1"/>
+      <c r="B2778" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C2778" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="2779">
       <c r="A2779" s="6" t="n">
         <v>44826.895833333336</v>
       </c>
-      <c r="B2779" s="1"/>
-      <c r="C2779" s="1"/>
+      <c r="B2779" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2779" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="2780">
       <c r="A2780" s="6" t="n">
         <v>44826.90625</v>
       </c>
-      <c r="B2780" s="1"/>
-      <c r="C2780" s="1"/>
+      <c r="B2780" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2780" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="2781">
       <c r="A2781" s="6" t="n">
         <v>44826.916666666664</v>
       </c>
-      <c r="B2781" s="1"/>
-      <c r="C2781" s="1"/>
+      <c r="B2781" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C2781" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="2782">
       <c r="A2782" s="6" t="n">
         <v>44826.927083333336</v>
       </c>
-      <c r="B2782" s="1"/>
-      <c r="C2782" s="1"/>
+      <c r="B2782" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2782" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="2783">
       <c r="A2783" s="6" t="n">
         <v>44826.9375</v>
       </c>
-      <c r="B2783" s="1"/>
-      <c r="C2783" s="1"/>
+      <c r="B2783" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2783" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="2784">
       <c r="A2784" s="6" t="n">
         <v>44826.947916666664</v>
       </c>
-      <c r="B2784" s="1"/>
-      <c r="C2784" s="1"/>
+      <c r="B2784" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2784" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="2785">
       <c r="A2785" s="6" t="n">
         <v>44826.958333333336</v>
       </c>
-      <c r="B2785" s="1"/>
-      <c r="C2785" s="1"/>
+      <c r="B2785" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2785" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="2786">
       <c r="A2786" s="6" t="n">
         <v>44826.96875</v>
       </c>
-      <c r="B2786" s="1"/>
-      <c r="C2786" s="1"/>
+      <c r="B2786" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2786" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="2787">
       <c r="A2787" s="6" t="n">
         <v>44826.979166666664</v>
       </c>
-      <c r="B2787" s="1"/>
-      <c r="C2787" s="1"/>
+      <c r="B2787" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2787" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="2788">
       <c r="A2788" s="6" t="n">
         <v>44826.989583333336</v>
       </c>
-      <c r="B2788" s="1"/>
-      <c r="C2788" s="1"/>
+      <c r="B2788" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2788" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2789">
+      <c r="A2789" s="6" t="n">
+        <v>44827.0</v>
+      </c>
+      <c r="B2789" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C2789" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2790">
+      <c r="A2790" s="6" t="n">
+        <v>44827.010416666664</v>
+      </c>
+      <c r="B2790" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2790" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2791">
+      <c r="A2791" s="6" t="n">
+        <v>44827.020833333336</v>
+      </c>
+      <c r="B2791" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2791" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2792">
+      <c r="A2792" s="6" t="n">
+        <v>44827.03125</v>
+      </c>
+      <c r="B2792" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2792" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2793">
+      <c r="A2793" s="6" t="n">
+        <v>44827.041666666664</v>
+      </c>
+      <c r="B2793" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2793" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2794">
+      <c r="A2794" s="6" t="n">
+        <v>44827.052083333336</v>
+      </c>
+      <c r="B2794" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2794" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2795">
+      <c r="A2795" s="6" t="n">
+        <v>44827.0625</v>
+      </c>
+      <c r="B2795" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2795" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2796">
+      <c r="A2796" s="6" t="n">
+        <v>44827.072916666664</v>
+      </c>
+      <c r="B2796" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2796" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2797">
+      <c r="A2797" s="6" t="n">
+        <v>44827.083333333336</v>
+      </c>
+      <c r="B2797" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2797" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2798">
+      <c r="A2798" s="6" t="n">
+        <v>44827.09375</v>
+      </c>
+      <c r="B2798" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2798" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2799">
+      <c r="A2799" s="6" t="n">
+        <v>44827.104166666664</v>
+      </c>
+      <c r="B2799" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2799" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2800">
+      <c r="A2800" s="6" t="n">
+        <v>44827.114583333336</v>
+      </c>
+      <c r="B2800" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2800" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2801">
+      <c r="A2801" s="6" t="n">
+        <v>44827.125</v>
+      </c>
+      <c r="B2801" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2801" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2802">
+      <c r="A2802" s="6" t="n">
+        <v>44827.135416666664</v>
+      </c>
+      <c r="B2802" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2802" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2803">
+      <c r="A2803" s="6" t="n">
+        <v>44827.145833333336</v>
+      </c>
+      <c r="B2803" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2803" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2804">
+      <c r="A2804" s="6" t="n">
+        <v>44827.15625</v>
+      </c>
+      <c r="B2804" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2804" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2805">
+      <c r="A2805" s="6" t="n">
+        <v>44827.166666666664</v>
+      </c>
+      <c r="B2805" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2805" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2806">
+      <c r="A2806" s="6" t="n">
+        <v>44827.177083333336</v>
+      </c>
+      <c r="B2806" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2806" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2807">
+      <c r="A2807" s="6" t="n">
+        <v>44827.1875</v>
+      </c>
+      <c r="B2807" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2807" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2808">
+      <c r="A2808" s="6" t="n">
+        <v>44827.197916666664</v>
+      </c>
+      <c r="B2808" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2808" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2809">
+      <c r="A2809" s="6" t="n">
+        <v>44827.208333333336</v>
+      </c>
+      <c r="B2809" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2809" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2810">
+      <c r="A2810" s="6" t="n">
+        <v>44827.21875</v>
+      </c>
+      <c r="B2810" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2810" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2811">
+      <c r="A2811" s="6" t="n">
+        <v>44827.229166666664</v>
+      </c>
+      <c r="B2811" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2811" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2812">
+      <c r="A2812" s="6" t="n">
+        <v>44827.239583333336</v>
+      </c>
+      <c r="B2812" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2812" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2813">
+      <c r="A2813" s="6" t="n">
+        <v>44827.25</v>
+      </c>
+      <c r="B2813" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2813" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2814">
+      <c r="A2814" s="6" t="n">
+        <v>44827.260416666664</v>
+      </c>
+      <c r="B2814" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2814" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2815">
+      <c r="A2815" s="6" t="n">
+        <v>44827.270833333336</v>
+      </c>
+      <c r="B2815" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2815" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2816">
+      <c r="A2816" s="6" t="n">
+        <v>44827.28125</v>
+      </c>
+      <c r="B2816" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2816" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2817">
+      <c r="A2817" s="6" t="n">
+        <v>44827.291666666664</v>
+      </c>
+      <c r="B2817" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2817" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2818">
+      <c r="A2818" s="6" t="n">
+        <v>44827.302083333336</v>
+      </c>
+      <c r="B2818" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2818" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2819">
+      <c r="A2819" s="6" t="n">
+        <v>44827.3125</v>
+      </c>
+      <c r="B2819" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2819" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2820">
+      <c r="A2820" s="6" t="n">
+        <v>44827.322916666664</v>
+      </c>
+      <c r="B2820" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C2820" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2821">
+      <c r="A2821" s="6" t="n">
+        <v>44827.333333333336</v>
+      </c>
+      <c r="B2821" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C2821" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2822">
+      <c r="A2822" s="6" t="n">
+        <v>44827.34375</v>
+      </c>
+      <c r="B2822" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C2822" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2823">
+      <c r="A2823" s="6" t="n">
+        <v>44827.354166666664</v>
+      </c>
+      <c r="B2823" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2823" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2824">
+      <c r="A2824" s="6" t="n">
+        <v>44827.364583333336</v>
+      </c>
+      <c r="B2824" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2824" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2825">
+      <c r="A2825" s="6" t="n">
+        <v>44827.375</v>
+      </c>
+      <c r="B2825" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2825" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2826">
+      <c r="A2826" s="6" t="n">
+        <v>44827.385416666664</v>
+      </c>
+      <c r="B2826" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2826" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2827">
+      <c r="A2827" s="6" t="n">
+        <v>44827.395833333336</v>
+      </c>
+      <c r="B2827" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2827" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="2828">
+      <c r="A2828" s="6" t="n">
+        <v>44827.40625</v>
+      </c>
+      <c r="B2828" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2828" s="1" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="2829">
+      <c r="A2829" s="6" t="n">
+        <v>44827.416666666664</v>
+      </c>
+      <c r="B2829" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2829" s="1" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="2830">
+      <c r="A2830" s="6" t="n">
+        <v>44827.427083333336</v>
+      </c>
+      <c r="B2830" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C2830" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2831">
+      <c r="A2831" s="6" t="n">
+        <v>44827.4375</v>
+      </c>
+      <c r="B2831" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2831" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="2832">
+      <c r="A2832" s="6" t="n">
+        <v>44827.447916666664</v>
+      </c>
+      <c r="B2832" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2832" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2833">
+      <c r="A2833" s="6" t="n">
+        <v>44827.458333333336</v>
+      </c>
+      <c r="B2833" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C2833" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="2834">
+      <c r="A2834" s="6" t="n">
+        <v>44827.46875</v>
+      </c>
+      <c r="B2834" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2834" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2835">
+      <c r="A2835" s="6" t="n">
+        <v>44827.479166666664</v>
+      </c>
+      <c r="B2835" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C2835" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="2836">
+      <c r="A2836" s="6" t="n">
+        <v>44827.489583333336</v>
+      </c>
+      <c r="B2836" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2836" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2837">
+      <c r="A2837" s="6" t="n">
+        <v>44827.5</v>
+      </c>
+      <c r="B2837" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2837" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2838">
+      <c r="A2838" s="6" t="n">
+        <v>44827.510416666664</v>
+      </c>
+      <c r="B2838" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2838" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2839">
+      <c r="A2839" s="6" t="n">
+        <v>44827.520833333336</v>
+      </c>
+      <c r="B2839" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C2839" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2840">
+      <c r="A2840" s="6" t="n">
+        <v>44827.53125</v>
+      </c>
+      <c r="B2840" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2840" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2841">
+      <c r="A2841" s="6" t="n">
+        <v>44827.541666666664</v>
+      </c>
+      <c r="B2841" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C2841" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2842">
+      <c r="A2842" s="6" t="n">
+        <v>44827.552083333336</v>
+      </c>
+      <c r="B2842" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C2842" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2843">
+      <c r="A2843" s="6" t="n">
+        <v>44827.5625</v>
+      </c>
+      <c r="B2843" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2843" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2844">
+      <c r="A2844" s="6" t="n">
+        <v>44827.572916666664</v>
+      </c>
+      <c r="B2844" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2844" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="2845">
+      <c r="A2845" s="6" t="n">
+        <v>44827.583333333336</v>
+      </c>
+      <c r="B2845" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C2845" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="2846">
+      <c r="A2846" s="6" t="n">
+        <v>44827.59375</v>
+      </c>
+      <c r="B2846" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C2846" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2847">
+      <c r="A2847" s="6" t="n">
+        <v>44827.604166666664</v>
+      </c>
+      <c r="B2847" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2847" s="1" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="2848">
+      <c r="A2848" s="6" t="n">
+        <v>44827.614583333336</v>
+      </c>
+      <c r="B2848" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2848" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2849">
+      <c r="A2849" s="6" t="n">
+        <v>44827.625</v>
+      </c>
+      <c r="B2849" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C2849" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="2850">
+      <c r="A2850" s="6" t="n">
+        <v>44827.635416666664</v>
+      </c>
+      <c r="B2850" s="1" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C2850" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2851">
+      <c r="A2851" s="6" t="n">
+        <v>44827.645833333336</v>
+      </c>
+      <c r="B2851" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C2851" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2852">
+      <c r="A2852" s="6" t="n">
+        <v>44827.65625</v>
+      </c>
+      <c r="B2852" s="1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C2852" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2853">
+      <c r="A2853" s="6" t="n">
+        <v>44827.666666666664</v>
+      </c>
+      <c r="B2853" s="1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C2853" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2854">
+      <c r="A2854" s="6" t="n">
+        <v>44827.677083333336</v>
+      </c>
+      <c r="B2854" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2854" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="2855">
+      <c r="A2855" s="6" t="n">
+        <v>44827.6875</v>
+      </c>
+      <c r="B2855" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2855" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2856">
+      <c r="A2856" s="6" t="n">
+        <v>44827.697916666664</v>
+      </c>
+      <c r="B2856" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C2856" s="1" t="n">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="2857">
+      <c r="A2857" s="6" t="n">
+        <v>44827.708333333336</v>
+      </c>
+      <c r="B2857" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C2857" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2858">
+      <c r="A2858" s="6" t="n">
+        <v>44827.71875</v>
+      </c>
+      <c r="B2858" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C2858" s="1" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="2859">
+      <c r="A2859" s="6" t="n">
+        <v>44827.729166666664</v>
+      </c>
+      <c r="B2859" s="1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C2859" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2860">
+      <c r="A2860" s="6" t="n">
+        <v>44827.739583333336</v>
+      </c>
+      <c r="B2860" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2860" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="2861">
+      <c r="A2861" s="6" t="n">
+        <v>44827.75</v>
+      </c>
+      <c r="B2861" s="1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C2861" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2862">
+      <c r="A2862" s="6" t="n">
+        <v>44827.760416666664</v>
+      </c>
+      <c r="B2862" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2862" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2863">
+      <c r="A2863" s="6" t="n">
+        <v>44827.770833333336</v>
+      </c>
+      <c r="B2863" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C2863" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2864">
+      <c r="A2864" s="6" t="n">
+        <v>44827.78125</v>
+      </c>
+      <c r="B2864" s="1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C2864" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2865">
+      <c r="A2865" s="6" t="n">
+        <v>44827.791666666664</v>
+      </c>
+      <c r="B2865" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2865" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2866">
+      <c r="A2866" s="6" t="n">
+        <v>44827.802083333336</v>
+      </c>
+      <c r="B2866" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C2866" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2867">
+      <c r="A2867" s="6" t="n">
+        <v>44827.8125</v>
+      </c>
+      <c r="B2867" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C2867" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2868">
+      <c r="A2868" s="6" t="n">
+        <v>44827.822916666664</v>
+      </c>
+      <c r="B2868" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2868" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2869">
+      <c r="A2869" s="6" t="n">
+        <v>44827.833333333336</v>
+      </c>
+      <c r="B2869" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2869" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2870">
+      <c r="A2870" s="6" t="n">
+        <v>44827.84375</v>
+      </c>
+      <c r="B2870" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C2870" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2871">
+      <c r="A2871" s="6" t="n">
+        <v>44827.854166666664</v>
+      </c>
+      <c r="B2871" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2871" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2872">
+      <c r="A2872" s="6" t="n">
+        <v>44827.864583333336</v>
+      </c>
+      <c r="B2872" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2872" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2873">
+      <c r="A2873" s="6" t="n">
+        <v>44827.875</v>
+      </c>
+      <c r="B2873" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2873" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2874">
+      <c r="A2874" s="6" t="n">
+        <v>44827.885416666664</v>
+      </c>
+      <c r="B2874" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2874" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2875">
+      <c r="A2875" s="6" t="n">
+        <v>44827.895833333336</v>
+      </c>
+      <c r="B2875" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2875" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2876">
+      <c r="A2876" s="6" t="n">
+        <v>44827.90625</v>
+      </c>
+      <c r="B2876" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2876" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2877">
+      <c r="A2877" s="6" t="n">
+        <v>44827.916666666664</v>
+      </c>
+      <c r="B2877" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2877" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2878">
+      <c r="A2878" s="6" t="n">
+        <v>44827.927083333336</v>
+      </c>
+      <c r="B2878" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2878" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2879">
+      <c r="A2879" s="6" t="n">
+        <v>44827.9375</v>
+      </c>
+      <c r="B2879" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C2879" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2880">
+      <c r="A2880" s="6" t="n">
+        <v>44827.947916666664</v>
+      </c>
+      <c r="B2880" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2880" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2881">
+      <c r="A2881" s="6" t="n">
+        <v>44827.958333333336</v>
+      </c>
+      <c r="B2881" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2881" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2882">
+      <c r="A2882" s="6" t="n">
+        <v>44827.96875</v>
+      </c>
+      <c r="B2882" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2882" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2883">
+      <c r="A2883" s="6" t="n">
+        <v>44827.979166666664</v>
+      </c>
+      <c r="B2883" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2883" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2884">
+      <c r="A2884" s="6" t="n">
+        <v>44827.989583333336</v>
+      </c>
+      <c r="B2884" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2884" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2885">
+      <c r="A2885" s="6" t="n">
+        <v>44828.0</v>
+      </c>
+      <c r="B2885" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C2885" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2886">
+      <c r="A2886" s="6" t="n">
+        <v>44828.010416666664</v>
+      </c>
+      <c r="B2886" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2886" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2887">
+      <c r="A2887" s="6" t="n">
+        <v>44828.020833333336</v>
+      </c>
+      <c r="B2887" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2887" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2888">
+      <c r="A2888" s="6" t="n">
+        <v>44828.03125</v>
+      </c>
+      <c r="B2888" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C2888" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2889">
+      <c r="A2889" s="6" t="n">
+        <v>44828.041666666664</v>
+      </c>
+      <c r="B2889" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2889" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2890">
+      <c r="A2890" s="6" t="n">
+        <v>44828.052083333336</v>
+      </c>
+      <c r="B2890" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2890" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2891">
+      <c r="A2891" s="6" t="n">
+        <v>44828.0625</v>
+      </c>
+      <c r="B2891" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C2891" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2892">
+      <c r="A2892" s="6" t="n">
+        <v>44828.072916666664</v>
+      </c>
+      <c r="B2892" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2892" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2893">
+      <c r="A2893" s="6" t="n">
+        <v>44828.083333333336</v>
+      </c>
+      <c r="B2893" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2893" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2894">
+      <c r="A2894" s="6" t="n">
+        <v>44828.09375</v>
+      </c>
+      <c r="B2894" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2894" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2895">
+      <c r="A2895" s="6" t="n">
+        <v>44828.104166666664</v>
+      </c>
+      <c r="B2895" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2895" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2896">
+      <c r="A2896" s="6" t="n">
+        <v>44828.114583333336</v>
+      </c>
+      <c r="B2896" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2896" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2897">
+      <c r="A2897" s="6" t="n">
+        <v>44828.125</v>
+      </c>
+      <c r="B2897" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2897" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2898">
+      <c r="A2898" s="6" t="n">
+        <v>44828.135416666664</v>
+      </c>
+      <c r="B2898" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2898" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2899">
+      <c r="A2899" s="6" t="n">
+        <v>44828.145833333336</v>
+      </c>
+      <c r="B2899" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2899" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2900">
+      <c r="A2900" s="6" t="n">
+        <v>44828.15625</v>
+      </c>
+      <c r="B2900" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2900" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2901">
+      <c r="A2901" s="6" t="n">
+        <v>44828.166666666664</v>
+      </c>
+      <c r="B2901" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2901" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2902">
+      <c r="A2902" s="6" t="n">
+        <v>44828.177083333336</v>
+      </c>
+      <c r="B2902" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2902" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2903">
+      <c r="A2903" s="6" t="n">
+        <v>44828.1875</v>
+      </c>
+      <c r="B2903" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2903" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2904">
+      <c r="A2904" s="6" t="n">
+        <v>44828.197916666664</v>
+      </c>
+      <c r="B2904" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2904" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2905">
+      <c r="A2905" s="6" t="n">
+        <v>44828.208333333336</v>
+      </c>
+      <c r="B2905" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2905" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2906">
+      <c r="A2906" s="6" t="n">
+        <v>44828.21875</v>
+      </c>
+      <c r="B2906" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2906" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2907">
+      <c r="A2907" s="6" t="n">
+        <v>44828.229166666664</v>
+      </c>
+      <c r="B2907" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2907" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2908">
+      <c r="A2908" s="6" t="n">
+        <v>44828.239583333336</v>
+      </c>
+      <c r="B2908" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2908" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2909">
+      <c r="A2909" s="6" t="n">
+        <v>44828.25</v>
+      </c>
+      <c r="B2909" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2909" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2910">
+      <c r="A2910" s="6" t="n">
+        <v>44828.260416666664</v>
+      </c>
+      <c r="B2910" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2910" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2911">
+      <c r="A2911" s="6" t="n">
+        <v>44828.270833333336</v>
+      </c>
+      <c r="B2911" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2911" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2912">
+      <c r="A2912" s="6" t="n">
+        <v>44828.28125</v>
+      </c>
+      <c r="B2912" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2912" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2913">
+      <c r="A2913" s="6" t="n">
+        <v>44828.291666666664</v>
+      </c>
+      <c r="B2913" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2913" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2914">
+      <c r="A2914" s="6" t="n">
+        <v>44828.302083333336</v>
+      </c>
+      <c r="B2914" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C2914" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2915">
+      <c r="A2915" s="6" t="n">
+        <v>44828.3125</v>
+      </c>
+      <c r="B2915" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2915" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2916">
+      <c r="A2916" s="6" t="n">
+        <v>44828.322916666664</v>
+      </c>
+      <c r="B2916" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2916" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2917">
+      <c r="A2917" s="6" t="n">
+        <v>44828.333333333336</v>
+      </c>
+      <c r="B2917" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2917" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="2918">
+      <c r="A2918" s="6" t="n">
+        <v>44828.34375</v>
+      </c>
+      <c r="B2918" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2918" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2919">
+      <c r="A2919" s="6" t="n">
+        <v>44828.354166666664</v>
+      </c>
+      <c r="B2919" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2919" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2920">
+      <c r="A2920" s="6" t="n">
+        <v>44828.364583333336</v>
+      </c>
+      <c r="B2920" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2920" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="2921">
+      <c r="A2921" s="6" t="n">
+        <v>44828.375</v>
+      </c>
+      <c r="B2921" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2921" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2922">
+      <c r="A2922" s="6" t="n">
+        <v>44828.385416666664</v>
+      </c>
+      <c r="B2922" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2922" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2923">
+      <c r="A2923" s="6" t="n">
+        <v>44828.395833333336</v>
+      </c>
+      <c r="B2923" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C2923" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2924">
+      <c r="A2924" s="6" t="n">
+        <v>44828.40625</v>
+      </c>
+      <c r="B2924" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C2924" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="2925">
+      <c r="A2925" s="6" t="n">
+        <v>44828.416666666664</v>
+      </c>
+      <c r="B2925" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2925" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="2926">
+      <c r="A2926" s="6" t="n">
+        <v>44828.427083333336</v>
+      </c>
+      <c r="B2926" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C2926" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2927">
+      <c r="A2927" s="6" t="n">
+        <v>44828.4375</v>
+      </c>
+      <c r="B2927" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C2927" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2928">
+      <c r="A2928" s="6" t="n">
+        <v>44828.447916666664</v>
+      </c>
+      <c r="B2928" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2928" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="2929">
+      <c r="A2929" s="6" t="n">
+        <v>44828.458333333336</v>
+      </c>
+      <c r="B2929" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2929" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2930">
+      <c r="A2930" s="6" t="n">
+        <v>44828.46875</v>
+      </c>
+      <c r="B2930" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2930" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="2931">
+      <c r="A2931" s="6" t="n">
+        <v>44828.479166666664</v>
+      </c>
+      <c r="B2931" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2931" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2932">
+      <c r="A2932" s="6" t="n">
+        <v>44828.489583333336</v>
+      </c>
+      <c r="B2932" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C2932" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="2933">
+      <c r="A2933" s="6" t="n">
+        <v>44828.5</v>
+      </c>
+      <c r="B2933" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C2933" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2934">
+      <c r="A2934" s="6" t="n">
+        <v>44828.510416666664</v>
+      </c>
+      <c r="B2934" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C2934" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2935">
+      <c r="A2935" s="6" t="n">
+        <v>44828.520833333336</v>
+      </c>
+      <c r="B2935" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2935" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2936">
+      <c r="A2936" s="6" t="n">
+        <v>44828.53125</v>
+      </c>
+      <c r="B2936" s="1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C2936" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2937">
+      <c r="A2937" s="6" t="n">
+        <v>44828.541666666664</v>
+      </c>
+      <c r="B2937" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2937" s="1" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="2938">
+      <c r="A2938" s="6" t="n">
+        <v>44828.552083333336</v>
+      </c>
+      <c r="B2938" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C2938" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2939">
+      <c r="A2939" s="6" t="n">
+        <v>44828.5625</v>
+      </c>
+      <c r="B2939" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C2939" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2940">
+      <c r="A2940" s="6" t="n">
+        <v>44828.572916666664</v>
+      </c>
+      <c r="B2940" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C2940" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2941">
+      <c r="A2941" s="6" t="n">
+        <v>44828.583333333336</v>
+      </c>
+      <c r="B2941" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C2941" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2942">
+      <c r="A2942" s="6" t="n">
+        <v>44828.59375</v>
+      </c>
+      <c r="B2942" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2942" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2943">
+      <c r="A2943" s="6" t="n">
+        <v>44828.604166666664</v>
+      </c>
+      <c r="B2943" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C2943" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2944">
+      <c r="A2944" s="6" t="n">
+        <v>44828.614583333336</v>
+      </c>
+      <c r="B2944" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2944" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2945">
+      <c r="A2945" s="6" t="n">
+        <v>44828.625</v>
+      </c>
+      <c r="B2945" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C2945" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2946">
+      <c r="A2946" s="6" t="n">
+        <v>44828.635416666664</v>
+      </c>
+      <c r="B2946" s="1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C2946" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2947">
+      <c r="A2947" s="6" t="n">
+        <v>44828.645833333336</v>
+      </c>
+      <c r="B2947" s="1" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="C2947" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2948">
+      <c r="A2948" s="6" t="n">
+        <v>44828.65625</v>
+      </c>
+      <c r="B2948" s="1" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="C2948" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2949">
+      <c r="A2949" s="6" t="n">
+        <v>44828.666666666664</v>
+      </c>
+      <c r="B2949" s="1" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="C2949" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="2950">
+      <c r="A2950" s="6" t="n">
+        <v>44828.677083333336</v>
+      </c>
+      <c r="B2950" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C2950" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2951">
+      <c r="A2951" s="6" t="n">
+        <v>44828.6875</v>
+      </c>
+      <c r="B2951" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C2951" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="2952">
+      <c r="A2952" s="6" t="n">
+        <v>44828.697916666664</v>
+      </c>
+      <c r="B2952" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C2952" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2953">
+      <c r="A2953" s="6" t="n">
+        <v>44828.708333333336</v>
+      </c>
+      <c r="B2953" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C2953" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="2954">
+      <c r="A2954" s="6" t="n">
+        <v>44828.71875</v>
+      </c>
+      <c r="B2954" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C2954" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="2955">
+      <c r="A2955" s="6" t="n">
+        <v>44828.729166666664</v>
+      </c>
+      <c r="B2955" s="1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C2955" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2956">
+      <c r="A2956" s="6" t="n">
+        <v>44828.739583333336</v>
+      </c>
+      <c r="B2956" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2956" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2957">
+      <c r="A2957" s="6" t="n">
+        <v>44828.75</v>
+      </c>
+      <c r="B2957" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C2957" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="2958">
+      <c r="A2958" s="6" t="n">
+        <v>44828.760416666664</v>
+      </c>
+      <c r="B2958" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2958" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2959">
+      <c r="A2959" s="6" t="n">
+        <v>44828.770833333336</v>
+      </c>
+      <c r="B2959" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2959" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2960">
+      <c r="A2960" s="6" t="n">
+        <v>44828.78125</v>
+      </c>
+      <c r="B2960" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2960" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2961">
+      <c r="A2961" s="6" t="n">
+        <v>44828.791666666664</v>
+      </c>
+      <c r="B2961" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2961" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2962">
+      <c r="A2962" s="6" t="n">
+        <v>44828.802083333336</v>
+      </c>
+      <c r="B2962" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2962" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2963">
+      <c r="A2963" s="6" t="n">
+        <v>44828.8125</v>
+      </c>
+      <c r="B2963" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C2963" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2964">
+      <c r="A2964" s="6" t="n">
+        <v>44828.822916666664</v>
+      </c>
+      <c r="B2964" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2964" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="2965">
+      <c r="A2965" s="6" t="n">
+        <v>44828.833333333336</v>
+      </c>
+      <c r="B2965" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C2965" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2966">
+      <c r="A2966" s="6" t="n">
+        <v>44828.84375</v>
+      </c>
+      <c r="B2966" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2966" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2967">
+      <c r="A2967" s="6" t="n">
+        <v>44828.854166666664</v>
+      </c>
+      <c r="B2967" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2967" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2968">
+      <c r="A2968" s="6" t="n">
+        <v>44828.864583333336</v>
+      </c>
+      <c r="B2968" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2968" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2969">
+      <c r="A2969" s="6" t="n">
+        <v>44828.875</v>
+      </c>
+      <c r="B2969" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2969" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="2970">
+      <c r="A2970" s="6" t="n">
+        <v>44828.885416666664</v>
+      </c>
+      <c r="B2970" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2970" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2971">
+      <c r="A2971" s="6" t="n">
+        <v>44828.895833333336</v>
+      </c>
+      <c r="B2971" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C2971" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2972">
+      <c r="A2972" s="6" t="n">
+        <v>44828.90625</v>
+      </c>
+      <c r="B2972" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2972" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2973">
+      <c r="A2973" s="6" t="n">
+        <v>44828.916666666664</v>
+      </c>
+      <c r="B2973" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C2973" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2974">
+      <c r="A2974" s="6" t="n">
+        <v>44828.927083333336</v>
+      </c>
+      <c r="B2974" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2974" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2975">
+      <c r="A2975" s="6" t="n">
+        <v>44828.9375</v>
+      </c>
+      <c r="B2975" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2975" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2976">
+      <c r="A2976" s="6" t="n">
+        <v>44828.947916666664</v>
+      </c>
+      <c r="B2976" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2976" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="2977">
+      <c r="A2977" s="6" t="n">
+        <v>44828.958333333336</v>
+      </c>
+      <c r="B2977" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2977" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2978">
+      <c r="A2978" s="6" t="n">
+        <v>44828.96875</v>
+      </c>
+      <c r="B2978" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2978" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2979">
+      <c r="A2979" s="6" t="n">
+        <v>44828.979166666664</v>
+      </c>
+      <c r="B2979" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2979" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2980">
+      <c r="A2980" s="6" t="n">
+        <v>44828.989583333336</v>
+      </c>
+      <c r="B2980" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2980" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2981">
+      <c r="A2981" s="6" t="n">
+        <v>44829.0</v>
+      </c>
+      <c r="B2981" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2981" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2982">
+      <c r="A2982" s="6" t="n">
+        <v>44829.010416666664</v>
+      </c>
+      <c r="B2982" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2982" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2983">
+      <c r="A2983" s="6" t="n">
+        <v>44829.020833333336</v>
+      </c>
+      <c r="B2983" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2983" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2984">
+      <c r="A2984" s="6" t="n">
+        <v>44829.03125</v>
+      </c>
+      <c r="B2984" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2984" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2985">
+      <c r="A2985" s="6" t="n">
+        <v>44829.041666666664</v>
+      </c>
+      <c r="B2985" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2985" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2986">
+      <c r="A2986" s="6" t="n">
+        <v>44829.052083333336</v>
+      </c>
+      <c r="B2986" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2986" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2987">
+      <c r="A2987" s="6" t="n">
+        <v>44829.0625</v>
+      </c>
+      <c r="B2987" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2987" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2988">
+      <c r="A2988" s="6" t="n">
+        <v>44829.072916666664</v>
+      </c>
+      <c r="B2988" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2988" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2989">
+      <c r="A2989" s="6" t="n">
+        <v>44829.083333333336</v>
+      </c>
+      <c r="B2989" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2989" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="2990">
+      <c r="A2990" s="6" t="n">
+        <v>44829.09375</v>
+      </c>
+      <c r="B2990" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2990" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2991">
+      <c r="A2991" s="6" t="n">
+        <v>44829.104166666664</v>
+      </c>
+      <c r="B2991" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2991" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2992">
+      <c r="A2992" s="6" t="n">
+        <v>44829.114583333336</v>
+      </c>
+      <c r="B2992" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C2992" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2993">
+      <c r="A2993" s="6" t="n">
+        <v>44829.125</v>
+      </c>
+      <c r="B2993" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2993" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2994">
+      <c r="A2994" s="6" t="n">
+        <v>44829.135416666664</v>
+      </c>
+      <c r="B2994" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2994" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2995">
+      <c r="A2995" s="6" t="n">
+        <v>44829.145833333336</v>
+      </c>
+      <c r="B2995" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2995" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2996">
+      <c r="A2996" s="6" t="n">
+        <v>44829.15625</v>
+      </c>
+      <c r="B2996" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2996" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2997">
+      <c r="A2997" s="6" t="n">
+        <v>44829.166666666664</v>
+      </c>
+      <c r="B2997" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2997" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2998">
+      <c r="A2998" s="6" t="n">
+        <v>44829.177083333336</v>
+      </c>
+      <c r="B2998" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2998" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2999">
+      <c r="A2999" s="6" t="n">
+        <v>44829.1875</v>
+      </c>
+      <c r="B2999" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2999" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3000">
+      <c r="A3000" s="6" t="n">
+        <v>44829.197916666664</v>
+      </c>
+      <c r="B3000" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3000" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3001">
+      <c r="A3001" s="6" t="n">
+        <v>44829.208333333336</v>
+      </c>
+      <c r="B3001" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3001" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3002">
+      <c r="A3002" s="6" t="n">
+        <v>44829.21875</v>
+      </c>
+      <c r="B3002" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3002" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3003">
+      <c r="A3003" s="6" t="n">
+        <v>44829.229166666664</v>
+      </c>
+      <c r="B3003" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3003" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3004">
+      <c r="A3004" s="6" t="n">
+        <v>44829.239583333336</v>
+      </c>
+      <c r="B3004" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3004" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3005">
+      <c r="A3005" s="6" t="n">
+        <v>44829.25</v>
+      </c>
+      <c r="B3005" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3005" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3006">
+      <c r="A3006" s="6" t="n">
+        <v>44829.260416666664</v>
+      </c>
+      <c r="B3006" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3006" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3007">
+      <c r="A3007" s="6" t="n">
+        <v>44829.270833333336</v>
+      </c>
+      <c r="B3007" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3007" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3008">
+      <c r="A3008" s="6" t="n">
+        <v>44829.28125</v>
+      </c>
+      <c r="B3008" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3008" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3009">
+      <c r="A3009" s="6" t="n">
+        <v>44829.291666666664</v>
+      </c>
+      <c r="B3009" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3009" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3010">
+      <c r="A3010" s="6" t="n">
+        <v>44829.302083333336</v>
+      </c>
+      <c r="B3010" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3010" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3011">
+      <c r="A3011" s="6" t="n">
+        <v>44829.3125</v>
+      </c>
+      <c r="B3011" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3011" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3012">
+      <c r="A3012" s="6" t="n">
+        <v>44829.322916666664</v>
+      </c>
+      <c r="B3012" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3012" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3013">
+      <c r="A3013" s="6" t="n">
+        <v>44829.333333333336</v>
+      </c>
+      <c r="B3013" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3013" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3014">
+      <c r="A3014" s="6" t="n">
+        <v>44829.34375</v>
+      </c>
+      <c r="B3014" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3014" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3015">
+      <c r="A3015" s="6" t="n">
+        <v>44829.354166666664</v>
+      </c>
+      <c r="B3015" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3015" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3016">
+      <c r="A3016" s="6" t="n">
+        <v>44829.364583333336</v>
+      </c>
+      <c r="B3016" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3016" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3017">
+      <c r="A3017" s="6" t="n">
+        <v>44829.375</v>
+      </c>
+      <c r="B3017" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3017" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3018">
+      <c r="A3018" s="6" t="n">
+        <v>44829.385416666664</v>
+      </c>
+      <c r="B3018" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3018" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3019">
+      <c r="A3019" s="6" t="n">
+        <v>44829.395833333336</v>
+      </c>
+      <c r="B3019" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3019" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3020">
+      <c r="A3020" s="6" t="n">
+        <v>44829.40625</v>
+      </c>
+      <c r="B3020" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3020" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3021">
+      <c r="A3021" s="6" t="n">
+        <v>44829.416666666664</v>
+      </c>
+      <c r="B3021" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3021" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3022">
+      <c r="A3022" s="6" t="n">
+        <v>44829.427083333336</v>
+      </c>
+      <c r="B3022" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3022" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3023">
+      <c r="A3023" s="6" t="n">
+        <v>44829.4375</v>
+      </c>
+      <c r="B3023" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3023" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3024">
+      <c r="A3024" s="6" t="n">
+        <v>44829.447916666664</v>
+      </c>
+      <c r="B3024" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3024" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3025">
+      <c r="A3025" s="6" t="n">
+        <v>44829.458333333336</v>
+      </c>
+      <c r="B3025" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C3025" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3026">
+      <c r="A3026" s="6" t="n">
+        <v>44829.46875</v>
+      </c>
+      <c r="B3026" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3026" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3027">
+      <c r="A3027" s="6" t="n">
+        <v>44829.479166666664</v>
+      </c>
+      <c r="B3027" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3027" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3028">
+      <c r="A3028" s="6" t="n">
+        <v>44829.489583333336</v>
+      </c>
+      <c r="B3028" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3028" s="1" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="3029">
+      <c r="A3029" s="6" t="n">
+        <v>44829.5</v>
+      </c>
+      <c r="B3029" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3029" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="3030">
+      <c r="A3030" s="6" t="n">
+        <v>44829.510416666664</v>
+      </c>
+      <c r="B3030" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3030" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3031">
+      <c r="A3031" s="6" t="n">
+        <v>44829.520833333336</v>
+      </c>
+      <c r="B3031" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3031" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3032">
+      <c r="A3032" s="6" t="n">
+        <v>44829.53125</v>
+      </c>
+      <c r="B3032" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C3032" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3033">
+      <c r="A3033" s="6" t="n">
+        <v>44829.541666666664</v>
+      </c>
+      <c r="B3033" s="1" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C3033" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3034">
+      <c r="A3034" s="6" t="n">
+        <v>44829.552083333336</v>
+      </c>
+      <c r="B3034" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C3034" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3035">
+      <c r="A3035" s="6" t="n">
+        <v>44829.5625</v>
+      </c>
+      <c r="B3035" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3035" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3036">
+      <c r="A3036" s="6" t="n">
+        <v>44829.572916666664</v>
+      </c>
+      <c r="B3036" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C3036" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3037">
+      <c r="A3037" s="6" t="n">
+        <v>44829.583333333336</v>
+      </c>
+      <c r="B3037" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3037" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="3038">
+      <c r="A3038" s="6" t="n">
+        <v>44829.59375</v>
+      </c>
+      <c r="B3038" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3038" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3039">
+      <c r="A3039" s="6" t="n">
+        <v>44829.604166666664</v>
+      </c>
+      <c r="B3039" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3039" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3040">
+      <c r="A3040" s="6" t="n">
+        <v>44829.614583333336</v>
+      </c>
+      <c r="B3040" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3040" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3041">
+      <c r="A3041" s="6" t="n">
+        <v>44829.625</v>
+      </c>
+      <c r="B3041" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C3041" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3042">
+      <c r="A3042" s="6" t="n">
+        <v>44829.635416666664</v>
+      </c>
+      <c r="B3042" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3042" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3043">
+      <c r="A3043" s="6" t="n">
+        <v>44829.645833333336</v>
+      </c>
+      <c r="B3043" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3043" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3044">
+      <c r="A3044" s="6" t="n">
+        <v>44829.65625</v>
+      </c>
+      <c r="B3044" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3044" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3045">
+      <c r="A3045" s="6" t="n">
+        <v>44829.666666666664</v>
+      </c>
+      <c r="B3045" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3045" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3046">
+      <c r="A3046" s="6" t="n">
+        <v>44829.677083333336</v>
+      </c>
+      <c r="B3046" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3046" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3047">
+      <c r="A3047" s="6" t="n">
+        <v>44829.6875</v>
+      </c>
+      <c r="B3047" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3047" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3048">
+      <c r="A3048" s="6" t="n">
+        <v>44829.697916666664</v>
+      </c>
+      <c r="B3048" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3048" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="3049">
+      <c r="A3049" s="6" t="n">
+        <v>44829.708333333336</v>
+      </c>
+      <c r="B3049" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3049" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3050">
+      <c r="A3050" s="6" t="n">
+        <v>44829.71875</v>
+      </c>
+      <c r="B3050" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3050" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3051">
+      <c r="A3051" s="6" t="n">
+        <v>44829.729166666664</v>
+      </c>
+      <c r="B3051" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3051" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3052">
+      <c r="A3052" s="6" t="n">
+        <v>44829.739583333336</v>
+      </c>
+      <c r="B3052" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C3052" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3053">
+      <c r="A3053" s="6" t="n">
+        <v>44829.75</v>
+      </c>
+      <c r="B3053" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3053" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3054">
+      <c r="A3054" s="6" t="n">
+        <v>44829.760416666664</v>
+      </c>
+      <c r="B3054" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C3054" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3055">
+      <c r="A3055" s="6" t="n">
+        <v>44829.770833333336</v>
+      </c>
+      <c r="B3055" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3055" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3056">
+      <c r="A3056" s="6" t="n">
+        <v>44829.78125</v>
+      </c>
+      <c r="B3056" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3056" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3057">
+      <c r="A3057" s="6" t="n">
+        <v>44829.791666666664</v>
+      </c>
+      <c r="B3057" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3057" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3058">
+      <c r="A3058" s="6" t="n">
+        <v>44829.802083333336</v>
+      </c>
+      <c r="B3058" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3058" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3059">
+      <c r="A3059" s="6" t="n">
+        <v>44829.8125</v>
+      </c>
+      <c r="B3059" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3059" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3060">
+      <c r="A3060" s="6" t="n">
+        <v>44829.822916666664</v>
+      </c>
+      <c r="B3060" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3060" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3061">
+      <c r="A3061" s="6" t="n">
+        <v>44829.833333333336</v>
+      </c>
+      <c r="B3061" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3061" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3062">
+      <c r="A3062" s="6" t="n">
+        <v>44829.84375</v>
+      </c>
+      <c r="B3062" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3062" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3063">
+      <c r="A3063" s="6" t="n">
+        <v>44829.854166666664</v>
+      </c>
+      <c r="B3063" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3063" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3064">
+      <c r="A3064" s="6" t="n">
+        <v>44829.864583333336</v>
+      </c>
+      <c r="B3064" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3064" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3065">
+      <c r="A3065" s="6" t="n">
+        <v>44829.875</v>
+      </c>
+      <c r="B3065" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3065" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3066">
+      <c r="A3066" s="6" t="n">
+        <v>44829.885416666664</v>
+      </c>
+      <c r="B3066" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3066" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3067">
+      <c r="A3067" s="6" t="n">
+        <v>44829.895833333336</v>
+      </c>
+      <c r="B3067" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3067" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3068">
+      <c r="A3068" s="6" t="n">
+        <v>44829.90625</v>
+      </c>
+      <c r="B3068" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3068" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3069">
+      <c r="A3069" s="6" t="n">
+        <v>44829.916666666664</v>
+      </c>
+      <c r="B3069" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3069" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3070">
+      <c r="A3070" s="6" t="n">
+        <v>44829.927083333336</v>
+      </c>
+      <c r="B3070" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3070" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3071">
+      <c r="A3071" s="6" t="n">
+        <v>44829.9375</v>
+      </c>
+      <c r="B3071" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3071" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3072">
+      <c r="A3072" s="6" t="n">
+        <v>44829.947916666664</v>
+      </c>
+      <c r="B3072" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3072" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3073">
+      <c r="A3073" s="6" t="n">
+        <v>44829.958333333336</v>
+      </c>
+      <c r="B3073" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3073" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3074">
+      <c r="A3074" s="6" t="n">
+        <v>44829.96875</v>
+      </c>
+      <c r="B3074" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3074" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3075">
+      <c r="A3075" s="6" t="n">
+        <v>44829.979166666664</v>
+      </c>
+      <c r="B3075" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3075" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3076">
+      <c r="A3076" s="6" t="n">
+        <v>44829.989583333336</v>
+      </c>
+      <c r="B3076" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3076" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3077">
+      <c r="A3077" s="6" t="n">
+        <v>44830.0</v>
+      </c>
+      <c r="B3077" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3077" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3078">
+      <c r="A3078" s="6" t="n">
+        <v>44830.010416666664</v>
+      </c>
+      <c r="B3078" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3078" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3079">
+      <c r="A3079" s="6" t="n">
+        <v>44830.020833333336</v>
+      </c>
+      <c r="B3079" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3079" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3080">
+      <c r="A3080" s="6" t="n">
+        <v>44830.03125</v>
+      </c>
+      <c r="B3080" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3080" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3081">
+      <c r="A3081" s="6" t="n">
+        <v>44830.041666666664</v>
+      </c>
+      <c r="B3081" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3081" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3082">
+      <c r="A3082" s="6" t="n">
+        <v>44830.052083333336</v>
+      </c>
+      <c r="B3082" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3082" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3083">
+      <c r="A3083" s="6" t="n">
+        <v>44830.0625</v>
+      </c>
+      <c r="B3083" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3083" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3084">
+      <c r="A3084" s="6" t="n">
+        <v>44830.072916666664</v>
+      </c>
+      <c r="B3084" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3084" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3085">
+      <c r="A3085" s="6" t="n">
+        <v>44830.083333333336</v>
+      </c>
+      <c r="B3085" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3085" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3086">
+      <c r="A3086" s="6" t="n">
+        <v>44830.09375</v>
+      </c>
+      <c r="B3086" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3086" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3087">
+      <c r="A3087" s="6" t="n">
+        <v>44830.104166666664</v>
+      </c>
+      <c r="B3087" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3087" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3088">
+      <c r="A3088" s="6" t="n">
+        <v>44830.114583333336</v>
+      </c>
+      <c r="B3088" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3088" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3089">
+      <c r="A3089" s="6" t="n">
+        <v>44830.125</v>
+      </c>
+      <c r="B3089" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3089" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3090">
+      <c r="A3090" s="6" t="n">
+        <v>44830.135416666664</v>
+      </c>
+      <c r="B3090" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3090" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3091">
+      <c r="A3091" s="6" t="n">
+        <v>44830.145833333336</v>
+      </c>
+      <c r="B3091" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3091" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3092">
+      <c r="A3092" s="6" t="n">
+        <v>44830.15625</v>
+      </c>
+      <c r="B3092" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3092" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3093">
+      <c r="A3093" s="6" t="n">
+        <v>44830.166666666664</v>
+      </c>
+      <c r="B3093" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3093" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3094">
+      <c r="A3094" s="6" t="n">
+        <v>44830.177083333336</v>
+      </c>
+      <c r="B3094" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3094" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3095">
+      <c r="A3095" s="6" t="n">
+        <v>44830.1875</v>
+      </c>
+      <c r="B3095" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3095" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3096">
+      <c r="A3096" s="6" t="n">
+        <v>44830.197916666664</v>
+      </c>
+      <c r="B3096" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3096" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3097">
+      <c r="A3097" s="6" t="n">
+        <v>44830.208333333336</v>
+      </c>
+      <c r="B3097" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3097" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3098">
+      <c r="A3098" s="6" t="n">
+        <v>44830.21875</v>
+      </c>
+      <c r="B3098" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3098" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3099">
+      <c r="A3099" s="6" t="n">
+        <v>44830.229166666664</v>
+      </c>
+      <c r="B3099" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3099" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3100">
+      <c r="A3100" s="6" t="n">
+        <v>44830.239583333336</v>
+      </c>
+      <c r="B3100" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3100" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3101">
+      <c r="A3101" s="6" t="n">
+        <v>44830.25</v>
+      </c>
+      <c r="B3101" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3101" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3102">
+      <c r="A3102" s="6" t="n">
+        <v>44830.260416666664</v>
+      </c>
+      <c r="B3102" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3102" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3103">
+      <c r="A3103" s="6" t="n">
+        <v>44830.270833333336</v>
+      </c>
+      <c r="B3103" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3103" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3104">
+      <c r="A3104" s="6" t="n">
+        <v>44830.28125</v>
+      </c>
+      <c r="B3104" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3104" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3105">
+      <c r="A3105" s="6" t="n">
+        <v>44830.291666666664</v>
+      </c>
+      <c r="B3105" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C3105" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3106">
+      <c r="A3106" s="6" t="n">
+        <v>44830.302083333336</v>
+      </c>
+      <c r="B3106" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3106" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3107">
+      <c r="A3107" s="6" t="n">
+        <v>44830.3125</v>
+      </c>
+      <c r="B3107" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C3107" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3108">
+      <c r="A3108" s="6" t="n">
+        <v>44830.322916666664</v>
+      </c>
+      <c r="B3108" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C3108" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3109">
+      <c r="A3109" s="6" t="n">
+        <v>44830.333333333336</v>
+      </c>
+      <c r="B3109" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C3109" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3110">
+      <c r="A3110" s="6" t="n">
+        <v>44830.34375</v>
+      </c>
+      <c r="B3110" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3110" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="3111">
+      <c r="A3111" s="6" t="n">
+        <v>44830.354166666664</v>
+      </c>
+      <c r="B3111" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3111" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3112">
+      <c r="A3112" s="6" t="n">
+        <v>44830.364583333336</v>
+      </c>
+      <c r="B3112" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3112" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3113">
+      <c r="A3113" s="6" t="n">
+        <v>44830.375</v>
+      </c>
+      <c r="B3113" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C3113" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3114">
+      <c r="A3114" s="6" t="n">
+        <v>44830.385416666664</v>
+      </c>
+      <c r="B3114" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3114" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3115">
+      <c r="A3115" s="6" t="n">
+        <v>44830.395833333336</v>
+      </c>
+      <c r="B3115" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3115" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="3116">
+      <c r="A3116" s="6" t="n">
+        <v>44830.40625</v>
+      </c>
+      <c r="B3116" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3116" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3117">
+      <c r="A3117" s="6" t="n">
+        <v>44830.416666666664</v>
+      </c>
+      <c r="B3117" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3117" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3118">
+      <c r="A3118" s="6" t="n">
+        <v>44830.427083333336</v>
+      </c>
+      <c r="B3118" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3118" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3119">
+      <c r="A3119" s="6" t="n">
+        <v>44830.4375</v>
+      </c>
+      <c r="B3119" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C3119" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3120">
+      <c r="A3120" s="6" t="n">
+        <v>44830.447916666664</v>
+      </c>
+      <c r="B3120" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3120" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3121">
+      <c r="A3121" s="6" t="n">
+        <v>44830.458333333336</v>
+      </c>
+      <c r="B3121" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3121" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3122">
+      <c r="A3122" s="6" t="n">
+        <v>44830.46875</v>
+      </c>
+      <c r="B3122" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3122" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3123">
+      <c r="A3123" s="6" t="n">
+        <v>44830.479166666664</v>
+      </c>
+      <c r="B3123" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C3123" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="3124">
+      <c r="A3124" s="6" t="n">
+        <v>44830.489583333336</v>
+      </c>
+      <c r="B3124" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3124" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3125">
+      <c r="A3125" s="6" t="n">
+        <v>44830.5</v>
+      </c>
+      <c r="B3125" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3125" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3126">
+      <c r="A3126" s="6" t="n">
+        <v>44830.510416666664</v>
+      </c>
+      <c r="B3126" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C3126" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3127">
+      <c r="A3127" s="6" t="n">
+        <v>44830.520833333336</v>
+      </c>
+      <c r="B3127" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C3127" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3128">
+      <c r="A3128" s="6" t="n">
+        <v>44830.53125</v>
+      </c>
+      <c r="B3128" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C3128" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3129">
+      <c r="A3129" s="6" t="n">
+        <v>44830.541666666664</v>
+      </c>
+      <c r="B3129" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3129" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3130">
+      <c r="A3130" s="6" t="n">
+        <v>44830.552083333336</v>
+      </c>
+      <c r="B3130" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3130" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3131">
+      <c r="A3131" s="6" t="n">
+        <v>44830.5625</v>
+      </c>
+      <c r="B3131" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3131" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3132">
+      <c r="A3132" s="6" t="n">
+        <v>44830.572916666664</v>
+      </c>
+      <c r="B3132" s="1"/>
+      <c r="C3132" s="1"/>
+    </row>
+    <row r="3133">
+      <c r="A3133" s="6" t="n">
+        <v>44830.583333333336</v>
+      </c>
+      <c r="B3133" s="1"/>
+      <c r="C3133" s="1"/>
+    </row>
+    <row r="3134">
+      <c r="A3134" s="6" t="n">
+        <v>44830.59375</v>
+      </c>
+      <c r="B3134" s="1"/>
+      <c r="C3134" s="1"/>
+    </row>
+    <row r="3135">
+      <c r="A3135" s="6" t="n">
+        <v>44830.604166666664</v>
+      </c>
+      <c r="B3135" s="1"/>
+      <c r="C3135" s="1"/>
+    </row>
+    <row r="3136">
+      <c r="A3136" s="6" t="n">
+        <v>44830.614583333336</v>
+      </c>
+      <c r="B3136" s="1"/>
+      <c r="C3136" s="1"/>
+    </row>
+    <row r="3137">
+      <c r="A3137" s="6" t="n">
+        <v>44830.625</v>
+      </c>
+      <c r="B3137" s="1"/>
+      <c r="C3137" s="1"/>
+    </row>
+    <row r="3138">
+      <c r="A3138" s="6" t="n">
+        <v>44830.635416666664</v>
+      </c>
+      <c r="B3138" s="1"/>
+      <c r="C3138" s="1"/>
+    </row>
+    <row r="3139">
+      <c r="A3139" s="6" t="n">
+        <v>44830.645833333336</v>
+      </c>
+      <c r="B3139" s="1"/>
+      <c r="C3139" s="1"/>
+    </row>
+    <row r="3140">
+      <c r="A3140" s="6" t="n">
+        <v>44830.65625</v>
+      </c>
+      <c r="B3140" s="1"/>
+      <c r="C3140" s="1"/>
+    </row>
+    <row r="3141">
+      <c r="A3141" s="6" t="n">
+        <v>44830.666666666664</v>
+      </c>
+      <c r="B3141" s="1"/>
+      <c r="C3141" s="1"/>
+    </row>
+    <row r="3142">
+      <c r="A3142" s="6" t="n">
+        <v>44830.677083333336</v>
+      </c>
+      <c r="B3142" s="1"/>
+      <c r="C3142" s="1"/>
+    </row>
+    <row r="3143">
+      <c r="A3143" s="6" t="n">
+        <v>44830.6875</v>
+      </c>
+      <c r="B3143" s="1"/>
+      <c r="C3143" s="1"/>
+    </row>
+    <row r="3144">
+      <c r="A3144" s="6" t="n">
+        <v>44830.697916666664</v>
+      </c>
+      <c r="B3144" s="1"/>
+      <c r="C3144" s="1"/>
+    </row>
+    <row r="3145">
+      <c r="A3145" s="6" t="n">
+        <v>44830.708333333336</v>
+      </c>
+      <c r="B3145" s="1"/>
+      <c r="C3145" s="1"/>
+    </row>
+    <row r="3146">
+      <c r="A3146" s="6" t="n">
+        <v>44830.71875</v>
+      </c>
+      <c r="B3146" s="1"/>
+      <c r="C3146" s="1"/>
+    </row>
+    <row r="3147">
+      <c r="A3147" s="6" t="n">
+        <v>44830.729166666664</v>
+      </c>
+      <c r="B3147" s="1"/>
+      <c r="C3147" s="1"/>
+    </row>
+    <row r="3148">
+      <c r="A3148" s="6" t="n">
+        <v>44830.739583333336</v>
+      </c>
+      <c r="B3148" s="1"/>
+      <c r="C3148" s="1"/>
+    </row>
+    <row r="3149">
+      <c r="A3149" s="6" t="n">
+        <v>44830.75</v>
+      </c>
+      <c r="B3149" s="1"/>
+      <c r="C3149" s="1"/>
+    </row>
+    <row r="3150">
+      <c r="A3150" s="6" t="n">
+        <v>44830.760416666664</v>
+      </c>
+      <c r="B3150" s="1"/>
+      <c r="C3150" s="1"/>
+    </row>
+    <row r="3151">
+      <c r="A3151" s="6" t="n">
+        <v>44830.770833333336</v>
+      </c>
+      <c r="B3151" s="1"/>
+      <c r="C3151" s="1"/>
+    </row>
+    <row r="3152">
+      <c r="A3152" s="6" t="n">
+        <v>44830.78125</v>
+      </c>
+      <c r="B3152" s="1"/>
+      <c r="C3152" s="1"/>
+    </row>
+    <row r="3153">
+      <c r="A3153" s="6" t="n">
+        <v>44830.791666666664</v>
+      </c>
+      <c r="B3153" s="1"/>
+      <c r="C3153" s="1"/>
+    </row>
+    <row r="3154">
+      <c r="A3154" s="6" t="n">
+        <v>44830.802083333336</v>
+      </c>
+      <c r="B3154" s="1"/>
+      <c r="C3154" s="1"/>
+    </row>
+    <row r="3155">
+      <c r="A3155" s="6" t="n">
+        <v>44830.8125</v>
+      </c>
+      <c r="B3155" s="1"/>
+      <c r="C3155" s="1"/>
+    </row>
+    <row r="3156">
+      <c r="A3156" s="6" t="n">
+        <v>44830.822916666664</v>
+      </c>
+      <c r="B3156" s="1"/>
+      <c r="C3156" s="1"/>
+    </row>
+    <row r="3157">
+      <c r="A3157" s="6" t="n">
+        <v>44830.833333333336</v>
+      </c>
+      <c r="B3157" s="1"/>
+      <c r="C3157" s="1"/>
+    </row>
+    <row r="3158">
+      <c r="A3158" s="6" t="n">
+        <v>44830.84375</v>
+      </c>
+      <c r="B3158" s="1"/>
+      <c r="C3158" s="1"/>
+    </row>
+    <row r="3159">
+      <c r="A3159" s="6" t="n">
+        <v>44830.854166666664</v>
+      </c>
+      <c r="B3159" s="1"/>
+      <c r="C3159" s="1"/>
+    </row>
+    <row r="3160">
+      <c r="A3160" s="6" t="n">
+        <v>44830.864583333336</v>
+      </c>
+      <c r="B3160" s="1"/>
+      <c r="C3160" s="1"/>
+    </row>
+    <row r="3161">
+      <c r="A3161" s="6" t="n">
+        <v>44830.875</v>
+      </c>
+      <c r="B3161" s="1"/>
+      <c r="C3161" s="1"/>
+    </row>
+    <row r="3162">
+      <c r="A3162" s="6" t="n">
+        <v>44830.885416666664</v>
+      </c>
+      <c r="B3162" s="1"/>
+      <c r="C3162" s="1"/>
+    </row>
+    <row r="3163">
+      <c r="A3163" s="6" t="n">
+        <v>44830.895833333336</v>
+      </c>
+      <c r="B3163" s="1"/>
+      <c r="C3163" s="1"/>
+    </row>
+    <row r="3164">
+      <c r="A3164" s="6" t="n">
+        <v>44830.90625</v>
+      </c>
+      <c r="B3164" s="1"/>
+      <c r="C3164" s="1"/>
+    </row>
+    <row r="3165">
+      <c r="A3165" s="6" t="n">
+        <v>44830.916666666664</v>
+      </c>
+      <c r="B3165" s="1"/>
+      <c r="C3165" s="1"/>
+    </row>
+    <row r="3166">
+      <c r="A3166" s="6" t="n">
+        <v>44830.927083333336</v>
+      </c>
+      <c r="B3166" s="1"/>
+      <c r="C3166" s="1"/>
+    </row>
+    <row r="3167">
+      <c r="A3167" s="6" t="n">
+        <v>44830.9375</v>
+      </c>
+      <c r="B3167" s="1"/>
+      <c r="C3167" s="1"/>
+    </row>
+    <row r="3168">
+      <c r="A3168" s="6" t="n">
+        <v>44830.947916666664</v>
+      </c>
+      <c r="B3168" s="1"/>
+      <c r="C3168" s="1"/>
+    </row>
+    <row r="3169">
+      <c r="A3169" s="6" t="n">
+        <v>44830.958333333336</v>
+      </c>
+      <c r="B3169" s="1"/>
+      <c r="C3169" s="1"/>
+    </row>
+    <row r="3170">
+      <c r="A3170" s="6" t="n">
+        <v>44830.96875</v>
+      </c>
+      <c r="B3170" s="1"/>
+      <c r="C3170" s="1"/>
+    </row>
+    <row r="3171">
+      <c r="A3171" s="6" t="n">
+        <v>44830.979166666664</v>
+      </c>
+      <c r="B3171" s="1"/>
+      <c r="C3171" s="1"/>
+    </row>
+    <row r="3172">
+      <c r="A3172" s="6" t="n">
+        <v>44830.989583333336</v>
+      </c>
+      <c r="B3172" s="1"/>
+      <c r="C3172" s="1"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
Update Ann Arbor counter data.
</commit_message>
<xml_diff>
--- a/data/export_data_domain_7992.xlsx
+++ b/data/export_data_domain_7992.xlsx
@@ -34572,288 +34572,2384 @@
       <c r="A3132" s="6" t="n">
         <v>44830.572916666664</v>
       </c>
-      <c r="B3132" s="1"/>
-      <c r="C3132" s="1"/>
+      <c r="B3132" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C3132" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="3133">
       <c r="A3133" s="6" t="n">
         <v>44830.583333333336</v>
       </c>
-      <c r="B3133" s="1"/>
-      <c r="C3133" s="1"/>
+      <c r="B3133" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C3133" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="3134">
       <c r="A3134" s="6" t="n">
         <v>44830.59375</v>
       </c>
-      <c r="B3134" s="1"/>
-      <c r="C3134" s="1"/>
+      <c r="B3134" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C3134" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="3135">
       <c r="A3135" s="6" t="n">
         <v>44830.604166666664</v>
       </c>
-      <c r="B3135" s="1"/>
-      <c r="C3135" s="1"/>
+      <c r="B3135" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C3135" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="3136">
       <c r="A3136" s="6" t="n">
         <v>44830.614583333336</v>
       </c>
-      <c r="B3136" s="1"/>
-      <c r="C3136" s="1"/>
+      <c r="B3136" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3136" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="3137">
       <c r="A3137" s="6" t="n">
         <v>44830.625</v>
       </c>
-      <c r="B3137" s="1"/>
-      <c r="C3137" s="1"/>
+      <c r="B3137" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3137" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="3138">
       <c r="A3138" s="6" t="n">
         <v>44830.635416666664</v>
       </c>
-      <c r="B3138" s="1"/>
-      <c r="C3138" s="1"/>
+      <c r="B3138" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C3138" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="3139">
       <c r="A3139" s="6" t="n">
         <v>44830.645833333336</v>
       </c>
-      <c r="B3139" s="1"/>
-      <c r="C3139" s="1"/>
+      <c r="B3139" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3139" s="1" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="3140">
       <c r="A3140" s="6" t="n">
         <v>44830.65625</v>
       </c>
-      <c r="B3140" s="1"/>
-      <c r="C3140" s="1"/>
+      <c r="B3140" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C3140" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="3141">
       <c r="A3141" s="6" t="n">
         <v>44830.666666666664</v>
       </c>
-      <c r="B3141" s="1"/>
-      <c r="C3141" s="1"/>
+      <c r="B3141" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3141" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="3142">
       <c r="A3142" s="6" t="n">
         <v>44830.677083333336</v>
       </c>
-      <c r="B3142" s="1"/>
-      <c r="C3142" s="1"/>
+      <c r="B3142" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3142" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="3143">
       <c r="A3143" s="6" t="n">
         <v>44830.6875</v>
       </c>
-      <c r="B3143" s="1"/>
-      <c r="C3143" s="1"/>
+      <c r="B3143" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C3143" s="1" t="n">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="3144">
       <c r="A3144" s="6" t="n">
         <v>44830.697916666664</v>
       </c>
-      <c r="B3144" s="1"/>
-      <c r="C3144" s="1"/>
+      <c r="B3144" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C3144" s="1" t="n">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="3145">
       <c r="A3145" s="6" t="n">
         <v>44830.708333333336</v>
       </c>
-      <c r="B3145" s="1"/>
-      <c r="C3145" s="1"/>
+      <c r="B3145" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C3145" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="3146">
       <c r="A3146" s="6" t="n">
         <v>44830.71875</v>
       </c>
-      <c r="B3146" s="1"/>
-      <c r="C3146" s="1"/>
+      <c r="B3146" s="1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C3146" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="3147">
       <c r="A3147" s="6" t="n">
         <v>44830.729166666664</v>
       </c>
-      <c r="B3147" s="1"/>
-      <c r="C3147" s="1"/>
+      <c r="B3147" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C3147" s="1" t="n">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="3148">
       <c r="A3148" s="6" t="n">
         <v>44830.739583333336</v>
       </c>
-      <c r="B3148" s="1"/>
-      <c r="C3148" s="1"/>
+      <c r="B3148" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C3148" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="3149">
       <c r="A3149" s="6" t="n">
         <v>44830.75</v>
       </c>
-      <c r="B3149" s="1"/>
-      <c r="C3149" s="1"/>
+      <c r="B3149" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3149" s="1" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="3150">
       <c r="A3150" s="6" t="n">
         <v>44830.760416666664</v>
       </c>
-      <c r="B3150" s="1"/>
-      <c r="C3150" s="1"/>
+      <c r="B3150" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3150" s="1" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="3151">
       <c r="A3151" s="6" t="n">
         <v>44830.770833333336</v>
       </c>
-      <c r="B3151" s="1"/>
-      <c r="C3151" s="1"/>
+      <c r="B3151" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3151" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="3152">
       <c r="A3152" s="6" t="n">
         <v>44830.78125</v>
       </c>
-      <c r="B3152" s="1"/>
-      <c r="C3152" s="1"/>
+      <c r="B3152" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3152" s="1" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="3153">
       <c r="A3153" s="6" t="n">
         <v>44830.791666666664</v>
       </c>
-      <c r="B3153" s="1"/>
-      <c r="C3153" s="1"/>
+      <c r="B3153" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3153" s="1" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="3154">
       <c r="A3154" s="6" t="n">
         <v>44830.802083333336</v>
       </c>
-      <c r="B3154" s="1"/>
-      <c r="C3154" s="1"/>
+      <c r="B3154" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3154" s="1" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="3155">
       <c r="A3155" s="6" t="n">
         <v>44830.8125</v>
       </c>
-      <c r="B3155" s="1"/>
-      <c r="C3155" s="1"/>
+      <c r="B3155" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3155" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="3156">
       <c r="A3156" s="6" t="n">
         <v>44830.822916666664</v>
       </c>
-      <c r="B3156" s="1"/>
-      <c r="C3156" s="1"/>
+      <c r="B3156" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C3156" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="3157">
       <c r="A3157" s="6" t="n">
         <v>44830.833333333336</v>
       </c>
-      <c r="B3157" s="1"/>
-      <c r="C3157" s="1"/>
+      <c r="B3157" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C3157" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="3158">
       <c r="A3158" s="6" t="n">
         <v>44830.84375</v>
       </c>
-      <c r="B3158" s="1"/>
-      <c r="C3158" s="1"/>
+      <c r="B3158" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3158" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="3159">
       <c r="A3159" s="6" t="n">
         <v>44830.854166666664</v>
       </c>
-      <c r="B3159" s="1"/>
-      <c r="C3159" s="1"/>
+      <c r="B3159" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3159" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="3160">
       <c r="A3160" s="6" t="n">
         <v>44830.864583333336</v>
       </c>
-      <c r="B3160" s="1"/>
-      <c r="C3160" s="1"/>
+      <c r="B3160" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C3160" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="3161">
       <c r="A3161" s="6" t="n">
         <v>44830.875</v>
       </c>
-      <c r="B3161" s="1"/>
-      <c r="C3161" s="1"/>
+      <c r="B3161" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3161" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="3162">
       <c r="A3162" s="6" t="n">
         <v>44830.885416666664</v>
       </c>
-      <c r="B3162" s="1"/>
-      <c r="C3162" s="1"/>
+      <c r="B3162" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3162" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="3163">
       <c r="A3163" s="6" t="n">
         <v>44830.895833333336</v>
       </c>
-      <c r="B3163" s="1"/>
-      <c r="C3163" s="1"/>
+      <c r="B3163" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3163" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="3164">
       <c r="A3164" s="6" t="n">
         <v>44830.90625</v>
       </c>
-      <c r="B3164" s="1"/>
-      <c r="C3164" s="1"/>
+      <c r="B3164" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3164" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="3165">
       <c r="A3165" s="6" t="n">
         <v>44830.916666666664</v>
       </c>
-      <c r="B3165" s="1"/>
-      <c r="C3165" s="1"/>
+      <c r="B3165" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3165" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="3166">
       <c r="A3166" s="6" t="n">
         <v>44830.927083333336</v>
       </c>
-      <c r="B3166" s="1"/>
-      <c r="C3166" s="1"/>
+      <c r="B3166" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3166" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="3167">
       <c r="A3167" s="6" t="n">
         <v>44830.9375</v>
       </c>
-      <c r="B3167" s="1"/>
-      <c r="C3167" s="1"/>
+      <c r="B3167" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3167" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="3168">
       <c r="A3168" s="6" t="n">
         <v>44830.947916666664</v>
       </c>
-      <c r="B3168" s="1"/>
-      <c r="C3168" s="1"/>
+      <c r="B3168" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3168" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="3169">
       <c r="A3169" s="6" t="n">
         <v>44830.958333333336</v>
       </c>
-      <c r="B3169" s="1"/>
-      <c r="C3169" s="1"/>
+      <c r="B3169" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C3169" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="3170">
       <c r="A3170" s="6" t="n">
         <v>44830.96875</v>
       </c>
-      <c r="B3170" s="1"/>
-      <c r="C3170" s="1"/>
+      <c r="B3170" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3170" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="3171">
       <c r="A3171" s="6" t="n">
         <v>44830.979166666664</v>
       </c>
-      <c r="B3171" s="1"/>
-      <c r="C3171" s="1"/>
+      <c r="B3171" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3171" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="3172">
       <c r="A3172" s="6" t="n">
         <v>44830.989583333336</v>
       </c>
-      <c r="B3172" s="1"/>
-      <c r="C3172" s="1"/>
+      <c r="B3172" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C3172" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3173">
+      <c r="A3173" s="6" t="n">
+        <v>44831.0</v>
+      </c>
+      <c r="B3173" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3173" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3174">
+      <c r="A3174" s="6" t="n">
+        <v>44831.010416666664</v>
+      </c>
+      <c r="B3174" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3174" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3175">
+      <c r="A3175" s="6" t="n">
+        <v>44831.020833333336</v>
+      </c>
+      <c r="B3175" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3175" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3176">
+      <c r="A3176" s="6" t="n">
+        <v>44831.03125</v>
+      </c>
+      <c r="B3176" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3176" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3177">
+      <c r="A3177" s="6" t="n">
+        <v>44831.041666666664</v>
+      </c>
+      <c r="B3177" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3177" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3178">
+      <c r="A3178" s="6" t="n">
+        <v>44831.052083333336</v>
+      </c>
+      <c r="B3178" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3178" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3179">
+      <c r="A3179" s="6" t="n">
+        <v>44831.0625</v>
+      </c>
+      <c r="B3179" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3179" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3180">
+      <c r="A3180" s="6" t="n">
+        <v>44831.072916666664</v>
+      </c>
+      <c r="B3180" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3180" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3181">
+      <c r="A3181" s="6" t="n">
+        <v>44831.083333333336</v>
+      </c>
+      <c r="B3181" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3181" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3182">
+      <c r="A3182" s="6" t="n">
+        <v>44831.09375</v>
+      </c>
+      <c r="B3182" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3182" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3183">
+      <c r="A3183" s="6" t="n">
+        <v>44831.104166666664</v>
+      </c>
+      <c r="B3183" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3183" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3184">
+      <c r="A3184" s="6" t="n">
+        <v>44831.114583333336</v>
+      </c>
+      <c r="B3184" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3184" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3185">
+      <c r="A3185" s="6" t="n">
+        <v>44831.125</v>
+      </c>
+      <c r="B3185" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3185" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3186">
+      <c r="A3186" s="6" t="n">
+        <v>44831.135416666664</v>
+      </c>
+      <c r="B3186" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3186" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3187">
+      <c r="A3187" s="6" t="n">
+        <v>44831.145833333336</v>
+      </c>
+      <c r="B3187" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3187" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3188">
+      <c r="A3188" s="6" t="n">
+        <v>44831.15625</v>
+      </c>
+      <c r="B3188" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3188" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3189">
+      <c r="A3189" s="6" t="n">
+        <v>44831.166666666664</v>
+      </c>
+      <c r="B3189" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3189" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3190">
+      <c r="A3190" s="6" t="n">
+        <v>44831.177083333336</v>
+      </c>
+      <c r="B3190" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3190" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3191">
+      <c r="A3191" s="6" t="n">
+        <v>44831.1875</v>
+      </c>
+      <c r="B3191" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3191" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3192">
+      <c r="A3192" s="6" t="n">
+        <v>44831.197916666664</v>
+      </c>
+      <c r="B3192" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3192" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3193">
+      <c r="A3193" s="6" t="n">
+        <v>44831.208333333336</v>
+      </c>
+      <c r="B3193" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3193" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3194">
+      <c r="A3194" s="6" t="n">
+        <v>44831.21875</v>
+      </c>
+      <c r="B3194" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3194" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3195">
+      <c r="A3195" s="6" t="n">
+        <v>44831.229166666664</v>
+      </c>
+      <c r="B3195" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3195" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3196">
+      <c r="A3196" s="6" t="n">
+        <v>44831.239583333336</v>
+      </c>
+      <c r="B3196" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3196" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3197">
+      <c r="A3197" s="6" t="n">
+        <v>44831.25</v>
+      </c>
+      <c r="B3197" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3197" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3198">
+      <c r="A3198" s="6" t="n">
+        <v>44831.260416666664</v>
+      </c>
+      <c r="B3198" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3198" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3199">
+      <c r="A3199" s="6" t="n">
+        <v>44831.270833333336</v>
+      </c>
+      <c r="B3199" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3199" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3200">
+      <c r="A3200" s="6" t="n">
+        <v>44831.28125</v>
+      </c>
+      <c r="B3200" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3200" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3201">
+      <c r="A3201" s="6" t="n">
+        <v>44831.291666666664</v>
+      </c>
+      <c r="B3201" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3201" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3202">
+      <c r="A3202" s="6" t="n">
+        <v>44831.302083333336</v>
+      </c>
+      <c r="B3202" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3202" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3203">
+      <c r="A3203" s="6" t="n">
+        <v>44831.3125</v>
+      </c>
+      <c r="B3203" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C3203" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3204">
+      <c r="A3204" s="6" t="n">
+        <v>44831.322916666664</v>
+      </c>
+      <c r="B3204" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C3204" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3205">
+      <c r="A3205" s="6" t="n">
+        <v>44831.333333333336</v>
+      </c>
+      <c r="B3205" s="1" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C3205" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3206">
+      <c r="A3206" s="6" t="n">
+        <v>44831.34375</v>
+      </c>
+      <c r="B3206" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3206" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="3207">
+      <c r="A3207" s="6" t="n">
+        <v>44831.354166666664</v>
+      </c>
+      <c r="B3207" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C3207" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3208">
+      <c r="A3208" s="6" t="n">
+        <v>44831.364583333336</v>
+      </c>
+      <c r="B3208" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3208" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3209">
+      <c r="A3209" s="6" t="n">
+        <v>44831.375</v>
+      </c>
+      <c r="B3209" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C3209" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3210">
+      <c r="A3210" s="6" t="n">
+        <v>44831.385416666664</v>
+      </c>
+      <c r="B3210" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C3210" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="3211">
+      <c r="A3211" s="6" t="n">
+        <v>44831.395833333336</v>
+      </c>
+      <c r="B3211" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C3211" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3212">
+      <c r="A3212" s="6" t="n">
+        <v>44831.40625</v>
+      </c>
+      <c r="B3212" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3212" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3213">
+      <c r="A3213" s="6" t="n">
+        <v>44831.416666666664</v>
+      </c>
+      <c r="B3213" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C3213" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="3214">
+      <c r="A3214" s="6" t="n">
+        <v>44831.427083333336</v>
+      </c>
+      <c r="B3214" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3214" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3215">
+      <c r="A3215" s="6" t="n">
+        <v>44831.4375</v>
+      </c>
+      <c r="B3215" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3215" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3216">
+      <c r="A3216" s="6" t="n">
+        <v>44831.447916666664</v>
+      </c>
+      <c r="B3216" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3216" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3217">
+      <c r="A3217" s="6" t="n">
+        <v>44831.458333333336</v>
+      </c>
+      <c r="B3217" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3217" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3218">
+      <c r="A3218" s="6" t="n">
+        <v>44831.46875</v>
+      </c>
+      <c r="B3218" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C3218" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3219">
+      <c r="A3219" s="6" t="n">
+        <v>44831.479166666664</v>
+      </c>
+      <c r="B3219" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C3219" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3220">
+      <c r="A3220" s="6" t="n">
+        <v>44831.489583333336</v>
+      </c>
+      <c r="B3220" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3220" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3221">
+      <c r="A3221" s="6" t="n">
+        <v>44831.5</v>
+      </c>
+      <c r="B3221" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C3221" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="3222">
+      <c r="A3222" s="6" t="n">
+        <v>44831.510416666664</v>
+      </c>
+      <c r="B3222" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3222" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3223">
+      <c r="A3223" s="6" t="n">
+        <v>44831.520833333336</v>
+      </c>
+      <c r="B3223" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3223" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3224">
+      <c r="A3224" s="6" t="n">
+        <v>44831.53125</v>
+      </c>
+      <c r="B3224" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3224" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3225">
+      <c r="A3225" s="6" t="n">
+        <v>44831.541666666664</v>
+      </c>
+      <c r="B3225" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3225" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3226">
+      <c r="A3226" s="6" t="n">
+        <v>44831.552083333336</v>
+      </c>
+      <c r="B3226" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C3226" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3227">
+      <c r="A3227" s="6" t="n">
+        <v>44831.5625</v>
+      </c>
+      <c r="B3227" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3227" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3228">
+      <c r="A3228" s="6" t="n">
+        <v>44831.572916666664</v>
+      </c>
+      <c r="B3228" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3228" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3229">
+      <c r="A3229" s="6" t="n">
+        <v>44831.583333333336</v>
+      </c>
+      <c r="B3229" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C3229" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3230">
+      <c r="A3230" s="6" t="n">
+        <v>44831.59375</v>
+      </c>
+      <c r="B3230" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C3230" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3231">
+      <c r="A3231" s="6" t="n">
+        <v>44831.604166666664</v>
+      </c>
+      <c r="B3231" s="1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C3231" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3232">
+      <c r="A3232" s="6" t="n">
+        <v>44831.614583333336</v>
+      </c>
+      <c r="B3232" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C3232" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3233">
+      <c r="A3233" s="6" t="n">
+        <v>44831.625</v>
+      </c>
+      <c r="B3233" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C3233" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3234">
+      <c r="A3234" s="6" t="n">
+        <v>44831.635416666664</v>
+      </c>
+      <c r="B3234" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C3234" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3235">
+      <c r="A3235" s="6" t="n">
+        <v>44831.645833333336</v>
+      </c>
+      <c r="B3235" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3235" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3236">
+      <c r="A3236" s="6" t="n">
+        <v>44831.65625</v>
+      </c>
+      <c r="B3236" s="1" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C3236" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3237">
+      <c r="A3237" s="6" t="n">
+        <v>44831.666666666664</v>
+      </c>
+      <c r="B3237" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3237" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3238">
+      <c r="A3238" s="6" t="n">
+        <v>44831.677083333336</v>
+      </c>
+      <c r="B3238" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3238" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3239">
+      <c r="A3239" s="6" t="n">
+        <v>44831.6875</v>
+      </c>
+      <c r="B3239" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C3239" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="3240">
+      <c r="A3240" s="6" t="n">
+        <v>44831.697916666664</v>
+      </c>
+      <c r="B3240" s="1" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="C3240" s="1" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="3241">
+      <c r="A3241" s="6" t="n">
+        <v>44831.708333333336</v>
+      </c>
+      <c r="B3241" s="1" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="C3241" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="3242">
+      <c r="A3242" s="6" t="n">
+        <v>44831.71875</v>
+      </c>
+      <c r="B3242" s="1" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C3242" s="1" t="n">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="3243">
+      <c r="A3243" s="6" t="n">
+        <v>44831.729166666664</v>
+      </c>
+      <c r="B3243" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C3243" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3244">
+      <c r="A3244" s="6" t="n">
+        <v>44831.739583333336</v>
+      </c>
+      <c r="B3244" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C3244" s="1" t="n">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="3245">
+      <c r="A3245" s="6" t="n">
+        <v>44831.75</v>
+      </c>
+      <c r="B3245" s="1" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="C3245" s="1" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="3246">
+      <c r="A3246" s="6" t="n">
+        <v>44831.760416666664</v>
+      </c>
+      <c r="B3246" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3246" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3247">
+      <c r="A3247" s="6" t="n">
+        <v>44831.770833333336</v>
+      </c>
+      <c r="B3247" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C3247" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3248">
+      <c r="A3248" s="6" t="n">
+        <v>44831.78125</v>
+      </c>
+      <c r="B3248" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3248" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3249">
+      <c r="A3249" s="6" t="n">
+        <v>44831.791666666664</v>
+      </c>
+      <c r="B3249" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3249" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3250">
+      <c r="A3250" s="6" t="n">
+        <v>44831.802083333336</v>
+      </c>
+      <c r="B3250" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C3250" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3251">
+      <c r="A3251" s="6" t="n">
+        <v>44831.8125</v>
+      </c>
+      <c r="B3251" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3251" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3252">
+      <c r="A3252" s="6" t="n">
+        <v>44831.822916666664</v>
+      </c>
+      <c r="B3252" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C3252" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3253">
+      <c r="A3253" s="6" t="n">
+        <v>44831.833333333336</v>
+      </c>
+      <c r="B3253" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3253" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3254">
+      <c r="A3254" s="6" t="n">
+        <v>44831.84375</v>
+      </c>
+      <c r="B3254" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3254" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3255">
+      <c r="A3255" s="6" t="n">
+        <v>44831.854166666664</v>
+      </c>
+      <c r="B3255" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3255" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3256">
+      <c r="A3256" s="6" t="n">
+        <v>44831.864583333336</v>
+      </c>
+      <c r="B3256" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3256" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3257">
+      <c r="A3257" s="6" t="n">
+        <v>44831.875</v>
+      </c>
+      <c r="B3257" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3257" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3258">
+      <c r="A3258" s="6" t="n">
+        <v>44831.885416666664</v>
+      </c>
+      <c r="B3258" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C3258" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3259">
+      <c r="A3259" s="6" t="n">
+        <v>44831.895833333336</v>
+      </c>
+      <c r="B3259" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3259" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3260">
+      <c r="A3260" s="6" t="n">
+        <v>44831.90625</v>
+      </c>
+      <c r="B3260" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3260" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3261">
+      <c r="A3261" s="6" t="n">
+        <v>44831.916666666664</v>
+      </c>
+      <c r="B3261" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3261" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3262">
+      <c r="A3262" s="6" t="n">
+        <v>44831.927083333336</v>
+      </c>
+      <c r="B3262" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3262" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3263">
+      <c r="A3263" s="6" t="n">
+        <v>44831.9375</v>
+      </c>
+      <c r="B3263" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3263" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3264">
+      <c r="A3264" s="6" t="n">
+        <v>44831.947916666664</v>
+      </c>
+      <c r="B3264" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3264" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3265">
+      <c r="A3265" s="6" t="n">
+        <v>44831.958333333336</v>
+      </c>
+      <c r="B3265" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3265" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3266">
+      <c r="A3266" s="6" t="n">
+        <v>44831.96875</v>
+      </c>
+      <c r="B3266" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3266" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3267">
+      <c r="A3267" s="6" t="n">
+        <v>44831.979166666664</v>
+      </c>
+      <c r="B3267" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3267" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3268">
+      <c r="A3268" s="6" t="n">
+        <v>44831.989583333336</v>
+      </c>
+      <c r="B3268" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3268" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3269">
+      <c r="A3269" s="6" t="n">
+        <v>44832.0</v>
+      </c>
+      <c r="B3269" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3269" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3270">
+      <c r="A3270" s="6" t="n">
+        <v>44832.010416666664</v>
+      </c>
+      <c r="B3270" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3270" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3271">
+      <c r="A3271" s="6" t="n">
+        <v>44832.020833333336</v>
+      </c>
+      <c r="B3271" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3271" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3272">
+      <c r="A3272" s="6" t="n">
+        <v>44832.03125</v>
+      </c>
+      <c r="B3272" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3272" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3273">
+      <c r="A3273" s="6" t="n">
+        <v>44832.041666666664</v>
+      </c>
+      <c r="B3273" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3273" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3274">
+      <c r="A3274" s="6" t="n">
+        <v>44832.052083333336</v>
+      </c>
+      <c r="B3274" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3274" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3275">
+      <c r="A3275" s="6" t="n">
+        <v>44832.0625</v>
+      </c>
+      <c r="B3275" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3275" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3276">
+      <c r="A3276" s="6" t="n">
+        <v>44832.072916666664</v>
+      </c>
+      <c r="B3276" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3276" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3277">
+      <c r="A3277" s="6" t="n">
+        <v>44832.083333333336</v>
+      </c>
+      <c r="B3277" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3277" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3278">
+      <c r="A3278" s="6" t="n">
+        <v>44832.09375</v>
+      </c>
+      <c r="B3278" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3278" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3279">
+      <c r="A3279" s="6" t="n">
+        <v>44832.104166666664</v>
+      </c>
+      <c r="B3279" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3279" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3280">
+      <c r="A3280" s="6" t="n">
+        <v>44832.114583333336</v>
+      </c>
+      <c r="B3280" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3280" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3281">
+      <c r="A3281" s="6" t="n">
+        <v>44832.125</v>
+      </c>
+      <c r="B3281" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3281" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3282">
+      <c r="A3282" s="6" t="n">
+        <v>44832.135416666664</v>
+      </c>
+      <c r="B3282" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3282" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3283">
+      <c r="A3283" s="6" t="n">
+        <v>44832.145833333336</v>
+      </c>
+      <c r="B3283" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3283" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3284">
+      <c r="A3284" s="6" t="n">
+        <v>44832.15625</v>
+      </c>
+      <c r="B3284" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3284" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3285">
+      <c r="A3285" s="6" t="n">
+        <v>44832.166666666664</v>
+      </c>
+      <c r="B3285" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3285" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3286">
+      <c r="A3286" s="6" t="n">
+        <v>44832.177083333336</v>
+      </c>
+      <c r="B3286" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3286" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3287">
+      <c r="A3287" s="6" t="n">
+        <v>44832.1875</v>
+      </c>
+      <c r="B3287" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3287" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3288">
+      <c r="A3288" s="6" t="n">
+        <v>44832.197916666664</v>
+      </c>
+      <c r="B3288" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3288" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3289">
+      <c r="A3289" s="6" t="n">
+        <v>44832.208333333336</v>
+      </c>
+      <c r="B3289" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3289" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3290">
+      <c r="A3290" s="6" t="n">
+        <v>44832.21875</v>
+      </c>
+      <c r="B3290" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3290" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3291">
+      <c r="A3291" s="6" t="n">
+        <v>44832.229166666664</v>
+      </c>
+      <c r="B3291" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3291" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3292">
+      <c r="A3292" s="6" t="n">
+        <v>44832.239583333336</v>
+      </c>
+      <c r="B3292" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3292" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3293">
+      <c r="A3293" s="6" t="n">
+        <v>44832.25</v>
+      </c>
+      <c r="B3293" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3293" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3294">
+      <c r="A3294" s="6" t="n">
+        <v>44832.260416666664</v>
+      </c>
+      <c r="B3294" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3294" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3295">
+      <c r="A3295" s="6" t="n">
+        <v>44832.270833333336</v>
+      </c>
+      <c r="B3295" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3295" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3296">
+      <c r="A3296" s="6" t="n">
+        <v>44832.28125</v>
+      </c>
+      <c r="B3296" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3296" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3297">
+      <c r="A3297" s="6" t="n">
+        <v>44832.291666666664</v>
+      </c>
+      <c r="B3297" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3297" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3298">
+      <c r="A3298" s="6" t="n">
+        <v>44832.302083333336</v>
+      </c>
+      <c r="B3298" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3298" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3299">
+      <c r="A3299" s="6" t="n">
+        <v>44832.3125</v>
+      </c>
+      <c r="B3299" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C3299" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3300">
+      <c r="A3300" s="6" t="n">
+        <v>44832.322916666664</v>
+      </c>
+      <c r="B3300" s="1" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C3300" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3301">
+      <c r="A3301" s="6" t="n">
+        <v>44832.333333333336</v>
+      </c>
+      <c r="B3301" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3301" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3302">
+      <c r="A3302" s="6" t="n">
+        <v>44832.34375</v>
+      </c>
+      <c r="B3302" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C3302" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3303">
+      <c r="A3303" s="6" t="n">
+        <v>44832.354166666664</v>
+      </c>
+      <c r="B3303" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3303" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="3304">
+      <c r="A3304" s="6" t="n">
+        <v>44832.364583333336</v>
+      </c>
+      <c r="B3304" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C3304" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3305">
+      <c r="A3305" s="6" t="n">
+        <v>44832.375</v>
+      </c>
+      <c r="B3305" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3305" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3306">
+      <c r="A3306" s="6" t="n">
+        <v>44832.385416666664</v>
+      </c>
+      <c r="B3306" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3306" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3307">
+      <c r="A3307" s="6" t="n">
+        <v>44832.395833333336</v>
+      </c>
+      <c r="B3307" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3307" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3308">
+      <c r="A3308" s="6" t="n">
+        <v>44832.40625</v>
+      </c>
+      <c r="B3308" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C3308" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3309">
+      <c r="A3309" s="6" t="n">
+        <v>44832.416666666664</v>
+      </c>
+      <c r="B3309" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3309" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="3310">
+      <c r="A3310" s="6" t="n">
+        <v>44832.427083333336</v>
+      </c>
+      <c r="B3310" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3310" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3311">
+      <c r="A3311" s="6" t="n">
+        <v>44832.4375</v>
+      </c>
+      <c r="B3311" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3311" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3312">
+      <c r="A3312" s="6" t="n">
+        <v>44832.447916666664</v>
+      </c>
+      <c r="B3312" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3312" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="3313">
+      <c r="A3313" s="6" t="n">
+        <v>44832.458333333336</v>
+      </c>
+      <c r="B3313" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C3313" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3314">
+      <c r="A3314" s="6" t="n">
+        <v>44832.46875</v>
+      </c>
+      <c r="B3314" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3314" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3315">
+      <c r="A3315" s="6" t="n">
+        <v>44832.479166666664</v>
+      </c>
+      <c r="B3315" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3315" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3316">
+      <c r="A3316" s="6" t="n">
+        <v>44832.489583333336</v>
+      </c>
+      <c r="B3316" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C3316" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3317">
+      <c r="A3317" s="6" t="n">
+        <v>44832.5</v>
+      </c>
+      <c r="B3317" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3317" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3318">
+      <c r="A3318" s="6" t="n">
+        <v>44832.510416666664</v>
+      </c>
+      <c r="B3318" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C3318" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3319">
+      <c r="A3319" s="6" t="n">
+        <v>44832.520833333336</v>
+      </c>
+      <c r="B3319" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C3319" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3320">
+      <c r="A3320" s="6" t="n">
+        <v>44832.53125</v>
+      </c>
+      <c r="B3320" s="1"/>
+      <c r="C3320" s="1"/>
+    </row>
+    <row r="3321">
+      <c r="A3321" s="6" t="n">
+        <v>44832.541666666664</v>
+      </c>
+      <c r="B3321" s="1"/>
+      <c r="C3321" s="1"/>
+    </row>
+    <row r="3322">
+      <c r="A3322" s="6" t="n">
+        <v>44832.552083333336</v>
+      </c>
+      <c r="B3322" s="1"/>
+      <c r="C3322" s="1"/>
+    </row>
+    <row r="3323">
+      <c r="A3323" s="6" t="n">
+        <v>44832.5625</v>
+      </c>
+      <c r="B3323" s="1"/>
+      <c r="C3323" s="1"/>
+    </row>
+    <row r="3324">
+      <c r="A3324" s="6" t="n">
+        <v>44832.572916666664</v>
+      </c>
+      <c r="B3324" s="1"/>
+      <c r="C3324" s="1"/>
+    </row>
+    <row r="3325">
+      <c r="A3325" s="6" t="n">
+        <v>44832.583333333336</v>
+      </c>
+      <c r="B3325" s="1"/>
+      <c r="C3325" s="1"/>
+    </row>
+    <row r="3326">
+      <c r="A3326" s="6" t="n">
+        <v>44832.59375</v>
+      </c>
+      <c r="B3326" s="1"/>
+      <c r="C3326" s="1"/>
+    </row>
+    <row r="3327">
+      <c r="A3327" s="6" t="n">
+        <v>44832.604166666664</v>
+      </c>
+      <c r="B3327" s="1"/>
+      <c r="C3327" s="1"/>
+    </row>
+    <row r="3328">
+      <c r="A3328" s="6" t="n">
+        <v>44832.614583333336</v>
+      </c>
+      <c r="B3328" s="1"/>
+      <c r="C3328" s="1"/>
+    </row>
+    <row r="3329">
+      <c r="A3329" s="6" t="n">
+        <v>44832.625</v>
+      </c>
+      <c r="B3329" s="1"/>
+      <c r="C3329" s="1"/>
+    </row>
+    <row r="3330">
+      <c r="A3330" s="6" t="n">
+        <v>44832.635416666664</v>
+      </c>
+      <c r="B3330" s="1"/>
+      <c r="C3330" s="1"/>
+    </row>
+    <row r="3331">
+      <c r="A3331" s="6" t="n">
+        <v>44832.645833333336</v>
+      </c>
+      <c r="B3331" s="1"/>
+      <c r="C3331" s="1"/>
+    </row>
+    <row r="3332">
+      <c r="A3332" s="6" t="n">
+        <v>44832.65625</v>
+      </c>
+      <c r="B3332" s="1"/>
+      <c r="C3332" s="1"/>
+    </row>
+    <row r="3333">
+      <c r="A3333" s="6" t="n">
+        <v>44832.666666666664</v>
+      </c>
+      <c r="B3333" s="1"/>
+      <c r="C3333" s="1"/>
+    </row>
+    <row r="3334">
+      <c r="A3334" s="6" t="n">
+        <v>44832.677083333336</v>
+      </c>
+      <c r="B3334" s="1"/>
+      <c r="C3334" s="1"/>
+    </row>
+    <row r="3335">
+      <c r="A3335" s="6" t="n">
+        <v>44832.6875</v>
+      </c>
+      <c r="B3335" s="1"/>
+      <c r="C3335" s="1"/>
+    </row>
+    <row r="3336">
+      <c r="A3336" s="6" t="n">
+        <v>44832.697916666664</v>
+      </c>
+      <c r="B3336" s="1"/>
+      <c r="C3336" s="1"/>
+    </row>
+    <row r="3337">
+      <c r="A3337" s="6" t="n">
+        <v>44832.708333333336</v>
+      </c>
+      <c r="B3337" s="1"/>
+      <c r="C3337" s="1"/>
+    </row>
+    <row r="3338">
+      <c r="A3338" s="6" t="n">
+        <v>44832.71875</v>
+      </c>
+      <c r="B3338" s="1"/>
+      <c r="C3338" s="1"/>
+    </row>
+    <row r="3339">
+      <c r="A3339" s="6" t="n">
+        <v>44832.729166666664</v>
+      </c>
+      <c r="B3339" s="1"/>
+      <c r="C3339" s="1"/>
+    </row>
+    <row r="3340">
+      <c r="A3340" s="6" t="n">
+        <v>44832.739583333336</v>
+      </c>
+      <c r="B3340" s="1"/>
+      <c r="C3340" s="1"/>
+    </row>
+    <row r="3341">
+      <c r="A3341" s="6" t="n">
+        <v>44832.75</v>
+      </c>
+      <c r="B3341" s="1"/>
+      <c r="C3341" s="1"/>
+    </row>
+    <row r="3342">
+      <c r="A3342" s="6" t="n">
+        <v>44832.760416666664</v>
+      </c>
+      <c r="B3342" s="1"/>
+      <c r="C3342" s="1"/>
+    </row>
+    <row r="3343">
+      <c r="A3343" s="6" t="n">
+        <v>44832.770833333336</v>
+      </c>
+      <c r="B3343" s="1"/>
+      <c r="C3343" s="1"/>
+    </row>
+    <row r="3344">
+      <c r="A3344" s="6" t="n">
+        <v>44832.78125</v>
+      </c>
+      <c r="B3344" s="1"/>
+      <c r="C3344" s="1"/>
+    </row>
+    <row r="3345">
+      <c r="A3345" s="6" t="n">
+        <v>44832.791666666664</v>
+      </c>
+      <c r="B3345" s="1"/>
+      <c r="C3345" s="1"/>
+    </row>
+    <row r="3346">
+      <c r="A3346" s="6" t="n">
+        <v>44832.802083333336</v>
+      </c>
+      <c r="B3346" s="1"/>
+      <c r="C3346" s="1"/>
+    </row>
+    <row r="3347">
+      <c r="A3347" s="6" t="n">
+        <v>44832.8125</v>
+      </c>
+      <c r="B3347" s="1"/>
+      <c r="C3347" s="1"/>
+    </row>
+    <row r="3348">
+      <c r="A3348" s="6" t="n">
+        <v>44832.822916666664</v>
+      </c>
+      <c r="B3348" s="1"/>
+      <c r="C3348" s="1"/>
+    </row>
+    <row r="3349">
+      <c r="A3349" s="6" t="n">
+        <v>44832.833333333336</v>
+      </c>
+      <c r="B3349" s="1"/>
+      <c r="C3349" s="1"/>
+    </row>
+    <row r="3350">
+      <c r="A3350" s="6" t="n">
+        <v>44832.84375</v>
+      </c>
+      <c r="B3350" s="1"/>
+      <c r="C3350" s="1"/>
+    </row>
+    <row r="3351">
+      <c r="A3351" s="6" t="n">
+        <v>44832.854166666664</v>
+      </c>
+      <c r="B3351" s="1"/>
+      <c r="C3351" s="1"/>
+    </row>
+    <row r="3352">
+      <c r="A3352" s="6" t="n">
+        <v>44832.864583333336</v>
+      </c>
+      <c r="B3352" s="1"/>
+      <c r="C3352" s="1"/>
+    </row>
+    <row r="3353">
+      <c r="A3353" s="6" t="n">
+        <v>44832.875</v>
+      </c>
+      <c r="B3353" s="1"/>
+      <c r="C3353" s="1"/>
+    </row>
+    <row r="3354">
+      <c r="A3354" s="6" t="n">
+        <v>44832.885416666664</v>
+      </c>
+      <c r="B3354" s="1"/>
+      <c r="C3354" s="1"/>
+    </row>
+    <row r="3355">
+      <c r="A3355" s="6" t="n">
+        <v>44832.895833333336</v>
+      </c>
+      <c r="B3355" s="1"/>
+      <c r="C3355" s="1"/>
+    </row>
+    <row r="3356">
+      <c r="A3356" s="6" t="n">
+        <v>44832.90625</v>
+      </c>
+      <c r="B3356" s="1"/>
+      <c r="C3356" s="1"/>
+    </row>
+    <row r="3357">
+      <c r="A3357" s="6" t="n">
+        <v>44832.916666666664</v>
+      </c>
+      <c r="B3357" s="1"/>
+      <c r="C3357" s="1"/>
+    </row>
+    <row r="3358">
+      <c r="A3358" s="6" t="n">
+        <v>44832.927083333336</v>
+      </c>
+      <c r="B3358" s="1"/>
+      <c r="C3358" s="1"/>
+    </row>
+    <row r="3359">
+      <c r="A3359" s="6" t="n">
+        <v>44832.9375</v>
+      </c>
+      <c r="B3359" s="1"/>
+      <c r="C3359" s="1"/>
+    </row>
+    <row r="3360">
+      <c r="A3360" s="6" t="n">
+        <v>44832.947916666664</v>
+      </c>
+      <c r="B3360" s="1"/>
+      <c r="C3360" s="1"/>
+    </row>
+    <row r="3361">
+      <c r="A3361" s="6" t="n">
+        <v>44832.958333333336</v>
+      </c>
+      <c r="B3361" s="1"/>
+      <c r="C3361" s="1"/>
+    </row>
+    <row r="3362">
+      <c r="A3362" s="6" t="n">
+        <v>44832.96875</v>
+      </c>
+      <c r="B3362" s="1"/>
+      <c r="C3362" s="1"/>
+    </row>
+    <row r="3363">
+      <c r="A3363" s="6" t="n">
+        <v>44832.979166666664</v>
+      </c>
+      <c r="B3363" s="1"/>
+      <c r="C3363" s="1"/>
+    </row>
+    <row r="3364">
+      <c r="A3364" s="6" t="n">
+        <v>44832.989583333336</v>
+      </c>
+      <c r="B3364" s="1"/>
+      <c r="C3364" s="1"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
Add event note hover feature; Customize hover fields; other misc changes.
</commit_message>
<xml_diff>
--- a/data/export_data_domain_7992.xlsx
+++ b/data/export_data_domain_7992.xlsx
@@ -65031,393 +65031,4673 @@
       <c r="A5901" s="6" t="n">
         <v>44859.416666666664</v>
       </c>
-      <c r="B5901" s="1"/>
-      <c r="C5901" s="1"/>
+      <c r="B5901" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C5901" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="5902">
       <c r="A5902" s="6" t="n">
         <v>44859.427083333336</v>
       </c>
-      <c r="B5902" s="1"/>
-      <c r="C5902" s="1"/>
+      <c r="B5902" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C5902" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5903">
       <c r="A5903" s="6" t="n">
         <v>44859.4375</v>
       </c>
-      <c r="B5903" s="1"/>
-      <c r="C5903" s="1"/>
+      <c r="B5903" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C5903" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="5904">
       <c r="A5904" s="6" t="n">
         <v>44859.447916666664</v>
       </c>
-      <c r="B5904" s="1"/>
-      <c r="C5904" s="1"/>
+      <c r="B5904" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C5904" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="5905">
       <c r="A5905" s="6" t="n">
         <v>44859.458333333336</v>
       </c>
-      <c r="B5905" s="1"/>
-      <c r="C5905" s="1"/>
+      <c r="B5905" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C5905" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5906">
       <c r="A5906" s="6" t="n">
         <v>44859.46875</v>
       </c>
-      <c r="B5906" s="1"/>
-      <c r="C5906" s="1"/>
+      <c r="B5906" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C5906" s="1" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="5907">
       <c r="A5907" s="6" t="n">
         <v>44859.479166666664</v>
       </c>
-      <c r="B5907" s="1"/>
-      <c r="C5907" s="1"/>
+      <c r="B5907" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C5907" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5908">
       <c r="A5908" s="6" t="n">
         <v>44859.489583333336</v>
       </c>
-      <c r="B5908" s="1"/>
-      <c r="C5908" s="1"/>
+      <c r="B5908" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C5908" s="1" t="n">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="5909">
       <c r="A5909" s="6" t="n">
         <v>44859.5</v>
       </c>
-      <c r="B5909" s="1"/>
-      <c r="C5909" s="1"/>
+      <c r="B5909" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C5909" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="5910">
       <c r="A5910" s="6" t="n">
         <v>44859.510416666664</v>
       </c>
-      <c r="B5910" s="1"/>
-      <c r="C5910" s="1"/>
+      <c r="B5910" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C5910" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="5911">
       <c r="A5911" s="6" t="n">
         <v>44859.520833333336</v>
       </c>
-      <c r="B5911" s="1"/>
-      <c r="C5911" s="1"/>
+      <c r="B5911" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5911" s="1" t="n">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="5912">
       <c r="A5912" s="6" t="n">
         <v>44859.53125</v>
       </c>
-      <c r="B5912" s="1"/>
-      <c r="C5912" s="1"/>
+      <c r="B5912" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C5912" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="5913">
       <c r="A5913" s="6" t="n">
         <v>44859.541666666664</v>
       </c>
-      <c r="B5913" s="1"/>
-      <c r="C5913" s="1"/>
+      <c r="B5913" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C5913" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5914">
       <c r="A5914" s="6" t="n">
         <v>44859.552083333336</v>
       </c>
-      <c r="B5914" s="1"/>
-      <c r="C5914" s="1"/>
+      <c r="B5914" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5914" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5915">
       <c r="A5915" s="6" t="n">
         <v>44859.5625</v>
       </c>
-      <c r="B5915" s="1"/>
-      <c r="C5915" s="1"/>
+      <c r="B5915" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C5915" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="5916">
       <c r="A5916" s="6" t="n">
         <v>44859.572916666664</v>
       </c>
-      <c r="B5916" s="1"/>
-      <c r="C5916" s="1"/>
+      <c r="B5916" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5916" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5917">
       <c r="A5917" s="6" t="n">
         <v>44859.583333333336</v>
       </c>
-      <c r="B5917" s="1"/>
-      <c r="C5917" s="1"/>
+      <c r="B5917" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C5917" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5918">
       <c r="A5918" s="6" t="n">
         <v>44859.59375</v>
       </c>
-      <c r="B5918" s="1"/>
-      <c r="C5918" s="1"/>
+      <c r="B5918" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C5918" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="5919">
       <c r="A5919" s="6" t="n">
         <v>44859.604166666664</v>
       </c>
-      <c r="B5919" s="1"/>
-      <c r="C5919" s="1"/>
+      <c r="B5919" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C5919" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="5920">
       <c r="A5920" s="6" t="n">
         <v>44859.614583333336</v>
       </c>
-      <c r="B5920" s="1"/>
-      <c r="C5920" s="1"/>
+      <c r="B5920" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C5920" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="5921">
       <c r="A5921" s="6" t="n">
         <v>44859.625</v>
       </c>
-      <c r="B5921" s="1"/>
-      <c r="C5921" s="1"/>
+      <c r="B5921" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C5921" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5922">
       <c r="A5922" s="6" t="n">
         <v>44859.635416666664</v>
       </c>
-      <c r="B5922" s="1"/>
-      <c r="C5922" s="1"/>
+      <c r="B5922" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C5922" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5923">
       <c r="A5923" s="6" t="n">
         <v>44859.645833333336</v>
       </c>
-      <c r="B5923" s="1"/>
-      <c r="C5923" s="1"/>
+      <c r="B5923" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C5923" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5924">
       <c r="A5924" s="6" t="n">
         <v>44859.65625</v>
       </c>
-      <c r="B5924" s="1"/>
-      <c r="C5924" s="1"/>
+      <c r="B5924" s="1" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="C5924" s="1" t="n">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="5925">
       <c r="A5925" s="6" t="n">
         <v>44859.666666666664</v>
       </c>
-      <c r="B5925" s="1"/>
-      <c r="C5925" s="1"/>
+      <c r="B5925" s="1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C5925" s="1" t="n">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="5926">
       <c r="A5926" s="6" t="n">
         <v>44859.677083333336</v>
       </c>
-      <c r="B5926" s="1"/>
-      <c r="C5926" s="1"/>
+      <c r="B5926" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C5926" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5927">
       <c r="A5927" s="6" t="n">
         <v>44859.6875</v>
       </c>
-      <c r="B5927" s="1"/>
-      <c r="C5927" s="1"/>
+      <c r="B5927" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C5927" s="1" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="5928">
       <c r="A5928" s="6" t="n">
         <v>44859.697916666664</v>
       </c>
-      <c r="B5928" s="1"/>
-      <c r="C5928" s="1"/>
+      <c r="B5928" s="1" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="C5928" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5929">
       <c r="A5929" s="6" t="n">
         <v>44859.708333333336</v>
       </c>
-      <c r="B5929" s="1"/>
-      <c r="C5929" s="1"/>
+      <c r="B5929" s="1" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="C5929" s="1" t="n">
+        <v>5.0</v>
+      </c>
     </row>
     <row r="5930">
       <c r="A5930" s="6" t="n">
         <v>44859.71875</v>
       </c>
-      <c r="B5930" s="1"/>
-      <c r="C5930" s="1"/>
+      <c r="B5930" s="1" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C5930" s="1" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="5931">
       <c r="A5931" s="6" t="n">
         <v>44859.729166666664</v>
       </c>
-      <c r="B5931" s="1"/>
-      <c r="C5931" s="1"/>
+      <c r="B5931" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C5931" s="1" t="n">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="5932">
       <c r="A5932" s="6" t="n">
         <v>44859.739583333336</v>
       </c>
-      <c r="B5932" s="1"/>
-      <c r="C5932" s="1"/>
+      <c r="B5932" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C5932" s="1" t="n">
+        <v>7.0</v>
+      </c>
     </row>
     <row r="5933">
       <c r="A5933" s="6" t="n">
         <v>44859.75</v>
       </c>
-      <c r="B5933" s="1"/>
-      <c r="C5933" s="1"/>
+      <c r="B5933" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C5933" s="1" t="n">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="5934">
       <c r="A5934" s="6" t="n">
         <v>44859.760416666664</v>
       </c>
-      <c r="B5934" s="1"/>
-      <c r="C5934" s="1"/>
+      <c r="B5934" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C5934" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="5935">
       <c r="A5935" s="6" t="n">
         <v>44859.770833333336</v>
       </c>
-      <c r="B5935" s="1"/>
-      <c r="C5935" s="1"/>
+      <c r="B5935" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C5935" s="1" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="5936">
       <c r="A5936" s="6" t="n">
         <v>44859.78125</v>
       </c>
-      <c r="B5936" s="1"/>
-      <c r="C5936" s="1"/>
+      <c r="B5936" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C5936" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5937">
       <c r="A5937" s="6" t="n">
         <v>44859.791666666664</v>
       </c>
-      <c r="B5937" s="1"/>
-      <c r="C5937" s="1"/>
+      <c r="B5937" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5937" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5938">
       <c r="A5938" s="6" t="n">
         <v>44859.802083333336</v>
       </c>
-      <c r="B5938" s="1"/>
-      <c r="C5938" s="1"/>
+      <c r="B5938" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C5938" s="1" t="n">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="5939">
       <c r="A5939" s="6" t="n">
         <v>44859.8125</v>
       </c>
-      <c r="B5939" s="1"/>
-      <c r="C5939" s="1"/>
+      <c r="B5939" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C5939" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5940">
       <c r="A5940" s="6" t="n">
         <v>44859.822916666664</v>
       </c>
-      <c r="B5940" s="1"/>
-      <c r="C5940" s="1"/>
+      <c r="B5940" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5940" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="5941">
       <c r="A5941" s="6" t="n">
         <v>44859.833333333336</v>
       </c>
-      <c r="B5941" s="1"/>
-      <c r="C5941" s="1"/>
+      <c r="B5941" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C5941" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5942">
       <c r="A5942" s="6" t="n">
         <v>44859.84375</v>
       </c>
-      <c r="B5942" s="1"/>
-      <c r="C5942" s="1"/>
+      <c r="B5942" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C5942" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="5943">
       <c r="A5943" s="6" t="n">
         <v>44859.854166666664</v>
       </c>
-      <c r="B5943" s="1"/>
-      <c r="C5943" s="1"/>
+      <c r="B5943" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C5943" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5944">
       <c r="A5944" s="6" t="n">
         <v>44859.864583333336</v>
       </c>
-      <c r="B5944" s="1"/>
-      <c r="C5944" s="1"/>
+      <c r="B5944" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C5944" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5945">
       <c r="A5945" s="6" t="n">
         <v>44859.875</v>
       </c>
-      <c r="B5945" s="1"/>
-      <c r="C5945" s="1"/>
+      <c r="B5945" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C5945" s="1" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="5946">
       <c r="A5946" s="6" t="n">
         <v>44859.885416666664</v>
       </c>
-      <c r="B5946" s="1"/>
-      <c r="C5946" s="1"/>
+      <c r="B5946" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C5946" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5947">
       <c r="A5947" s="6" t="n">
         <v>44859.895833333336</v>
       </c>
-      <c r="B5947" s="1"/>
-      <c r="C5947" s="1"/>
+      <c r="B5947" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C5947" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5948">
       <c r="A5948" s="6" t="n">
         <v>44859.90625</v>
       </c>
-      <c r="B5948" s="1"/>
-      <c r="C5948" s="1"/>
+      <c r="B5948" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5948" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5949">
       <c r="A5949" s="6" t="n">
         <v>44859.916666666664</v>
       </c>
-      <c r="B5949" s="1"/>
-      <c r="C5949" s="1"/>
+      <c r="B5949" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5949" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5950">
       <c r="A5950" s="6" t="n">
         <v>44859.927083333336</v>
       </c>
-      <c r="B5950" s="1"/>
-      <c r="C5950" s="1"/>
+      <c r="B5950" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C5950" s="1" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="5951">
       <c r="A5951" s="6" t="n">
         <v>44859.9375</v>
       </c>
-      <c r="B5951" s="1"/>
-      <c r="C5951" s="1"/>
+      <c r="B5951" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C5951" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="5952">
       <c r="A5952" s="6" t="n">
         <v>44859.947916666664</v>
       </c>
-      <c r="B5952" s="1"/>
-      <c r="C5952" s="1"/>
+      <c r="B5952" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C5952" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5953">
       <c r="A5953" s="6" t="n">
         <v>44859.958333333336</v>
       </c>
-      <c r="B5953" s="1"/>
-      <c r="C5953" s="1"/>
+      <c r="B5953" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5953" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5954">
       <c r="A5954" s="6" t="n">
         <v>44859.96875</v>
       </c>
-      <c r="B5954" s="1"/>
-      <c r="C5954" s="1"/>
+      <c r="B5954" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C5954" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5955">
       <c r="A5955" s="6" t="n">
         <v>44859.979166666664</v>
       </c>
-      <c r="B5955" s="1"/>
-      <c r="C5955" s="1"/>
+      <c r="B5955" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5955" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5956">
       <c r="A5956" s="6" t="n">
         <v>44859.989583333336</v>
       </c>
-      <c r="B5956" s="1"/>
-      <c r="C5956" s="1"/>
+      <c r="B5956" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5956" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5957">
+      <c r="A5957" s="6" t="n">
+        <v>44860.0</v>
+      </c>
+      <c r="B5957" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5957" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5958">
+      <c r="A5958" s="6" t="n">
+        <v>44860.010416666664</v>
+      </c>
+      <c r="B5958" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5958" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5959">
+      <c r="A5959" s="6" t="n">
+        <v>44860.020833333336</v>
+      </c>
+      <c r="B5959" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5959" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5960">
+      <c r="A5960" s="6" t="n">
+        <v>44860.03125</v>
+      </c>
+      <c r="B5960" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5960" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5961">
+      <c r="A5961" s="6" t="n">
+        <v>44860.041666666664</v>
+      </c>
+      <c r="B5961" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5961" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5962">
+      <c r="A5962" s="6" t="n">
+        <v>44860.052083333336</v>
+      </c>
+      <c r="B5962" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5962" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5963">
+      <c r="A5963" s="6" t="n">
+        <v>44860.0625</v>
+      </c>
+      <c r="B5963" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5963" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5964">
+      <c r="A5964" s="6" t="n">
+        <v>44860.072916666664</v>
+      </c>
+      <c r="B5964" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C5964" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5965">
+      <c r="A5965" s="6" t="n">
+        <v>44860.083333333336</v>
+      </c>
+      <c r="B5965" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5965" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5966">
+      <c r="A5966" s="6" t="n">
+        <v>44860.09375</v>
+      </c>
+      <c r="B5966" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5966" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5967">
+      <c r="A5967" s="6" t="n">
+        <v>44860.104166666664</v>
+      </c>
+      <c r="B5967" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5967" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5968">
+      <c r="A5968" s="6" t="n">
+        <v>44860.114583333336</v>
+      </c>
+      <c r="B5968" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5968" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5969">
+      <c r="A5969" s="6" t="n">
+        <v>44860.125</v>
+      </c>
+      <c r="B5969" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5969" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5970">
+      <c r="A5970" s="6" t="n">
+        <v>44860.135416666664</v>
+      </c>
+      <c r="B5970" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5970" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5971">
+      <c r="A5971" s="6" t="n">
+        <v>44860.145833333336</v>
+      </c>
+      <c r="B5971" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5971" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5972">
+      <c r="A5972" s="6" t="n">
+        <v>44860.15625</v>
+      </c>
+      <c r="B5972" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5972" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5973">
+      <c r="A5973" s="6" t="n">
+        <v>44860.166666666664</v>
+      </c>
+      <c r="B5973" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5973" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5974">
+      <c r="A5974" s="6" t="n">
+        <v>44860.177083333336</v>
+      </c>
+      <c r="B5974" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5974" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5975">
+      <c r="A5975" s="6" t="n">
+        <v>44860.1875</v>
+      </c>
+      <c r="B5975" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5975" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5976">
+      <c r="A5976" s="6" t="n">
+        <v>44860.197916666664</v>
+      </c>
+      <c r="B5976" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5976" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5977">
+      <c r="A5977" s="6" t="n">
+        <v>44860.208333333336</v>
+      </c>
+      <c r="B5977" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5977" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5978">
+      <c r="A5978" s="6" t="n">
+        <v>44860.21875</v>
+      </c>
+      <c r="B5978" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5978" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5979">
+      <c r="A5979" s="6" t="n">
+        <v>44860.229166666664</v>
+      </c>
+      <c r="B5979" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5979" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5980">
+      <c r="A5980" s="6" t="n">
+        <v>44860.239583333336</v>
+      </c>
+      <c r="B5980" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5980" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5981">
+      <c r="A5981" s="6" t="n">
+        <v>44860.25</v>
+      </c>
+      <c r="B5981" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5981" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5982">
+      <c r="A5982" s="6" t="n">
+        <v>44860.260416666664</v>
+      </c>
+      <c r="B5982" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5982" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5983">
+      <c r="A5983" s="6" t="n">
+        <v>44860.270833333336</v>
+      </c>
+      <c r="B5983" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5983" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5984">
+      <c r="A5984" s="6" t="n">
+        <v>44860.28125</v>
+      </c>
+      <c r="B5984" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5984" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="5985">
+      <c r="A5985" s="6" t="n">
+        <v>44860.291666666664</v>
+      </c>
+      <c r="B5985" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5985" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5986">
+      <c r="A5986" s="6" t="n">
+        <v>44860.302083333336</v>
+      </c>
+      <c r="B5986" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5986" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="5987">
+      <c r="A5987" s="6" t="n">
+        <v>44860.3125</v>
+      </c>
+      <c r="B5987" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C5987" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5988">
+      <c r="A5988" s="6" t="n">
+        <v>44860.322916666664</v>
+      </c>
+      <c r="B5988" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C5988" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="5989">
+      <c r="A5989" s="6" t="n">
+        <v>44860.333333333336</v>
+      </c>
+      <c r="B5989" s="1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C5989" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="5990">
+      <c r="A5990" s="6" t="n">
+        <v>44860.34375</v>
+      </c>
+      <c r="B5990" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5990" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="5991">
+      <c r="A5991" s="6" t="n">
+        <v>44860.354166666664</v>
+      </c>
+      <c r="B5991" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C5991" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5992">
+      <c r="A5992" s="6" t="n">
+        <v>44860.364583333336</v>
+      </c>
+      <c r="B5992" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C5992" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="5993">
+      <c r="A5993" s="6" t="n">
+        <v>44860.375</v>
+      </c>
+      <c r="B5993" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5993" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="5994">
+      <c r="A5994" s="6" t="n">
+        <v>44860.385416666664</v>
+      </c>
+      <c r="B5994" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5994" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="5995">
+      <c r="A5995" s="6" t="n">
+        <v>44860.395833333336</v>
+      </c>
+      <c r="B5995" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C5995" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="5996">
+      <c r="A5996" s="6" t="n">
+        <v>44860.40625</v>
+      </c>
+      <c r="B5996" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C5996" s="1" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="5997">
+      <c r="A5997" s="6" t="n">
+        <v>44860.416666666664</v>
+      </c>
+      <c r="B5997" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5997" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5998">
+      <c r="A5998" s="6" t="n">
+        <v>44860.427083333336</v>
+      </c>
+      <c r="B5998" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C5998" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5999">
+      <c r="A5999" s="6" t="n">
+        <v>44860.4375</v>
+      </c>
+      <c r="B5999" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C5999" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6000">
+      <c r="A6000" s="6" t="n">
+        <v>44860.447916666664</v>
+      </c>
+      <c r="B6000" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6000" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6001">
+      <c r="A6001" s="6" t="n">
+        <v>44860.458333333336</v>
+      </c>
+      <c r="B6001" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6001" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6002">
+      <c r="A6002" s="6" t="n">
+        <v>44860.46875</v>
+      </c>
+      <c r="B6002" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6002" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6003">
+      <c r="A6003" s="6" t="n">
+        <v>44860.479166666664</v>
+      </c>
+      <c r="B6003" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6003" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6004">
+      <c r="A6004" s="6" t="n">
+        <v>44860.489583333336</v>
+      </c>
+      <c r="B6004" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6004" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6005">
+      <c r="A6005" s="6" t="n">
+        <v>44860.5</v>
+      </c>
+      <c r="B6005" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6005" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6006">
+      <c r="A6006" s="6" t="n">
+        <v>44860.510416666664</v>
+      </c>
+      <c r="B6006" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6006" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="6007">
+      <c r="A6007" s="6" t="n">
+        <v>44860.520833333336</v>
+      </c>
+      <c r="B6007" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6007" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6008">
+      <c r="A6008" s="6" t="n">
+        <v>44860.53125</v>
+      </c>
+      <c r="B6008" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6008" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6009">
+      <c r="A6009" s="6" t="n">
+        <v>44860.541666666664</v>
+      </c>
+      <c r="B6009" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6009" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6010">
+      <c r="A6010" s="6" t="n">
+        <v>44860.552083333336</v>
+      </c>
+      <c r="B6010" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6010" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6011">
+      <c r="A6011" s="6" t="n">
+        <v>44860.5625</v>
+      </c>
+      <c r="B6011" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6011" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6012">
+      <c r="A6012" s="6" t="n">
+        <v>44860.572916666664</v>
+      </c>
+      <c r="B6012" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6012" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6013">
+      <c r="A6013" s="6" t="n">
+        <v>44860.583333333336</v>
+      </c>
+      <c r="B6013" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6013" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6014">
+      <c r="A6014" s="6" t="n">
+        <v>44860.59375</v>
+      </c>
+      <c r="B6014" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6014" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6015">
+      <c r="A6015" s="6" t="n">
+        <v>44860.604166666664</v>
+      </c>
+      <c r="B6015" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6015" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6016">
+      <c r="A6016" s="6" t="n">
+        <v>44860.614583333336</v>
+      </c>
+      <c r="B6016" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6016" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6017">
+      <c r="A6017" s="6" t="n">
+        <v>44860.625</v>
+      </c>
+      <c r="B6017" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6017" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6018">
+      <c r="A6018" s="6" t="n">
+        <v>44860.635416666664</v>
+      </c>
+      <c r="B6018" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6018" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6019">
+      <c r="A6019" s="6" t="n">
+        <v>44860.645833333336</v>
+      </c>
+      <c r="B6019" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6019" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6020">
+      <c r="A6020" s="6" t="n">
+        <v>44860.65625</v>
+      </c>
+      <c r="B6020" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6020" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6021">
+      <c r="A6021" s="6" t="n">
+        <v>44860.666666666664</v>
+      </c>
+      <c r="B6021" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6021" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6022">
+      <c r="A6022" s="6" t="n">
+        <v>44860.677083333336</v>
+      </c>
+      <c r="B6022" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6022" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6023">
+      <c r="A6023" s="6" t="n">
+        <v>44860.6875</v>
+      </c>
+      <c r="B6023" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6023" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6024">
+      <c r="A6024" s="6" t="n">
+        <v>44860.697916666664</v>
+      </c>
+      <c r="B6024" s="1" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="C6024" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6025">
+      <c r="A6025" s="6" t="n">
+        <v>44860.708333333336</v>
+      </c>
+      <c r="B6025" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6025" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6026">
+      <c r="A6026" s="6" t="n">
+        <v>44860.71875</v>
+      </c>
+      <c r="B6026" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6026" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6027">
+      <c r="A6027" s="6" t="n">
+        <v>44860.729166666664</v>
+      </c>
+      <c r="B6027" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6027" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6028">
+      <c r="A6028" s="6" t="n">
+        <v>44860.739583333336</v>
+      </c>
+      <c r="B6028" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C6028" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6029">
+      <c r="A6029" s="6" t="n">
+        <v>44860.75</v>
+      </c>
+      <c r="B6029" s="1" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C6029" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6030">
+      <c r="A6030" s="6" t="n">
+        <v>44860.760416666664</v>
+      </c>
+      <c r="B6030" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6030" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6031">
+      <c r="A6031" s="6" t="n">
+        <v>44860.770833333336</v>
+      </c>
+      <c r="B6031" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6031" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6032">
+      <c r="A6032" s="6" t="n">
+        <v>44860.78125</v>
+      </c>
+      <c r="B6032" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6032" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6033">
+      <c r="A6033" s="6" t="n">
+        <v>44860.791666666664</v>
+      </c>
+      <c r="B6033" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6033" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6034">
+      <c r="A6034" s="6" t="n">
+        <v>44860.802083333336</v>
+      </c>
+      <c r="B6034" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6034" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6035">
+      <c r="A6035" s="6" t="n">
+        <v>44860.8125</v>
+      </c>
+      <c r="B6035" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6035" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6036">
+      <c r="A6036" s="6" t="n">
+        <v>44860.822916666664</v>
+      </c>
+      <c r="B6036" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6036" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6037">
+      <c r="A6037" s="6" t="n">
+        <v>44860.833333333336</v>
+      </c>
+      <c r="B6037" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6037" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6038">
+      <c r="A6038" s="6" t="n">
+        <v>44860.84375</v>
+      </c>
+      <c r="B6038" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6038" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6039">
+      <c r="A6039" s="6" t="n">
+        <v>44860.854166666664</v>
+      </c>
+      <c r="B6039" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6039" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6040">
+      <c r="A6040" s="6" t="n">
+        <v>44860.864583333336</v>
+      </c>
+      <c r="B6040" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6040" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6041">
+      <c r="A6041" s="6" t="n">
+        <v>44860.875</v>
+      </c>
+      <c r="B6041" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6041" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6042">
+      <c r="A6042" s="6" t="n">
+        <v>44860.885416666664</v>
+      </c>
+      <c r="B6042" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6042" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6043">
+      <c r="A6043" s="6" t="n">
+        <v>44860.895833333336</v>
+      </c>
+      <c r="B6043" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6043" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6044">
+      <c r="A6044" s="6" t="n">
+        <v>44860.90625</v>
+      </c>
+      <c r="B6044" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6044" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6045">
+      <c r="A6045" s="6" t="n">
+        <v>44860.916666666664</v>
+      </c>
+      <c r="B6045" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6045" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6046">
+      <c r="A6046" s="6" t="n">
+        <v>44860.927083333336</v>
+      </c>
+      <c r="B6046" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6046" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6047">
+      <c r="A6047" s="6" t="n">
+        <v>44860.9375</v>
+      </c>
+      <c r="B6047" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6047" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6048">
+      <c r="A6048" s="6" t="n">
+        <v>44860.947916666664</v>
+      </c>
+      <c r="B6048" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6048" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6049">
+      <c r="A6049" s="6" t="n">
+        <v>44860.958333333336</v>
+      </c>
+      <c r="B6049" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6049" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6050">
+      <c r="A6050" s="6" t="n">
+        <v>44860.96875</v>
+      </c>
+      <c r="B6050" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6050" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6051">
+      <c r="A6051" s="6" t="n">
+        <v>44860.979166666664</v>
+      </c>
+      <c r="B6051" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6051" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6052">
+      <c r="A6052" s="6" t="n">
+        <v>44860.989583333336</v>
+      </c>
+      <c r="B6052" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6052" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6053">
+      <c r="A6053" s="6" t="n">
+        <v>44861.0</v>
+      </c>
+      <c r="B6053" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6053" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6054">
+      <c r="A6054" s="6" t="n">
+        <v>44861.010416666664</v>
+      </c>
+      <c r="B6054" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6054" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6055">
+      <c r="A6055" s="6" t="n">
+        <v>44861.020833333336</v>
+      </c>
+      <c r="B6055" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6055" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6056">
+      <c r="A6056" s="6" t="n">
+        <v>44861.03125</v>
+      </c>
+      <c r="B6056" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6056" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6057">
+      <c r="A6057" s="6" t="n">
+        <v>44861.041666666664</v>
+      </c>
+      <c r="B6057" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6057" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6058">
+      <c r="A6058" s="6" t="n">
+        <v>44861.052083333336</v>
+      </c>
+      <c r="B6058" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6058" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6059">
+      <c r="A6059" s="6" t="n">
+        <v>44861.0625</v>
+      </c>
+      <c r="B6059" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6059" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6060">
+      <c r="A6060" s="6" t="n">
+        <v>44861.072916666664</v>
+      </c>
+      <c r="B6060" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6060" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6061">
+      <c r="A6061" s="6" t="n">
+        <v>44861.083333333336</v>
+      </c>
+      <c r="B6061" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6061" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6062">
+      <c r="A6062" s="6" t="n">
+        <v>44861.09375</v>
+      </c>
+      <c r="B6062" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6062" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6063">
+      <c r="A6063" s="6" t="n">
+        <v>44861.104166666664</v>
+      </c>
+      <c r="B6063" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6063" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6064">
+      <c r="A6064" s="6" t="n">
+        <v>44861.114583333336</v>
+      </c>
+      <c r="B6064" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6064" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6065">
+      <c r="A6065" s="6" t="n">
+        <v>44861.125</v>
+      </c>
+      <c r="B6065" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6065" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6066">
+      <c r="A6066" s="6" t="n">
+        <v>44861.135416666664</v>
+      </c>
+      <c r="B6066" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6066" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6067">
+      <c r="A6067" s="6" t="n">
+        <v>44861.145833333336</v>
+      </c>
+      <c r="B6067" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6067" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6068">
+      <c r="A6068" s="6" t="n">
+        <v>44861.15625</v>
+      </c>
+      <c r="B6068" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6068" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6069">
+      <c r="A6069" s="6" t="n">
+        <v>44861.166666666664</v>
+      </c>
+      <c r="B6069" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6069" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6070">
+      <c r="A6070" s="6" t="n">
+        <v>44861.177083333336</v>
+      </c>
+      <c r="B6070" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6070" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6071">
+      <c r="A6071" s="6" t="n">
+        <v>44861.1875</v>
+      </c>
+      <c r="B6071" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6071" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6072">
+      <c r="A6072" s="6" t="n">
+        <v>44861.197916666664</v>
+      </c>
+      <c r="B6072" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6072" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6073">
+      <c r="A6073" s="6" t="n">
+        <v>44861.208333333336</v>
+      </c>
+      <c r="B6073" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6073" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6074">
+      <c r="A6074" s="6" t="n">
+        <v>44861.21875</v>
+      </c>
+      <c r="B6074" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6074" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6075">
+      <c r="A6075" s="6" t="n">
+        <v>44861.229166666664</v>
+      </c>
+      <c r="B6075" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6075" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6076">
+      <c r="A6076" s="6" t="n">
+        <v>44861.239583333336</v>
+      </c>
+      <c r="B6076" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6076" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6077">
+      <c r="A6077" s="6" t="n">
+        <v>44861.25</v>
+      </c>
+      <c r="B6077" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6077" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6078">
+      <c r="A6078" s="6" t="n">
+        <v>44861.260416666664</v>
+      </c>
+      <c r="B6078" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6078" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6079">
+      <c r="A6079" s="6" t="n">
+        <v>44861.270833333336</v>
+      </c>
+      <c r="B6079" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6079" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6080">
+      <c r="A6080" s="6" t="n">
+        <v>44861.28125</v>
+      </c>
+      <c r="B6080" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6080" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6081">
+      <c r="A6081" s="6" t="n">
+        <v>44861.291666666664</v>
+      </c>
+      <c r="B6081" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6081" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6082">
+      <c r="A6082" s="6" t="n">
+        <v>44861.302083333336</v>
+      </c>
+      <c r="B6082" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6082" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6083">
+      <c r="A6083" s="6" t="n">
+        <v>44861.3125</v>
+      </c>
+      <c r="B6083" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6083" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6084">
+      <c r="A6084" s="6" t="n">
+        <v>44861.322916666664</v>
+      </c>
+      <c r="B6084" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6084" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6085">
+      <c r="A6085" s="6" t="n">
+        <v>44861.333333333336</v>
+      </c>
+      <c r="B6085" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6085" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6086">
+      <c r="A6086" s="6" t="n">
+        <v>44861.34375</v>
+      </c>
+      <c r="B6086" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6086" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="6087">
+      <c r="A6087" s="6" t="n">
+        <v>44861.354166666664</v>
+      </c>
+      <c r="B6087" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6087" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6088">
+      <c r="A6088" s="6" t="n">
+        <v>44861.364583333336</v>
+      </c>
+      <c r="B6088" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6088" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6089">
+      <c r="A6089" s="6" t="n">
+        <v>44861.375</v>
+      </c>
+      <c r="B6089" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6089" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6090">
+      <c r="A6090" s="6" t="n">
+        <v>44861.385416666664</v>
+      </c>
+      <c r="B6090" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6090" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="6091">
+      <c r="A6091" s="6" t="n">
+        <v>44861.395833333336</v>
+      </c>
+      <c r="B6091" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6091" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6092">
+      <c r="A6092" s="6" t="n">
+        <v>44861.40625</v>
+      </c>
+      <c r="B6092" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6092" s="1" t="n">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="6093">
+      <c r="A6093" s="6" t="n">
+        <v>44861.416666666664</v>
+      </c>
+      <c r="B6093" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6093" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6094">
+      <c r="A6094" s="6" t="n">
+        <v>44861.427083333336</v>
+      </c>
+      <c r="B6094" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6094" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6095">
+      <c r="A6095" s="6" t="n">
+        <v>44861.4375</v>
+      </c>
+      <c r="B6095" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6095" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6096">
+      <c r="A6096" s="6" t="n">
+        <v>44861.447916666664</v>
+      </c>
+      <c r="B6096" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6096" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6097">
+      <c r="A6097" s="6" t="n">
+        <v>44861.458333333336</v>
+      </c>
+      <c r="B6097" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6097" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6098">
+      <c r="A6098" s="6" t="n">
+        <v>44861.46875</v>
+      </c>
+      <c r="B6098" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6098" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6099">
+      <c r="A6099" s="6" t="n">
+        <v>44861.479166666664</v>
+      </c>
+      <c r="B6099" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6099" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6100">
+      <c r="A6100" s="6" t="n">
+        <v>44861.489583333336</v>
+      </c>
+      <c r="B6100" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6100" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6101">
+      <c r="A6101" s="6" t="n">
+        <v>44861.5</v>
+      </c>
+      <c r="B6101" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6101" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6102">
+      <c r="A6102" s="6" t="n">
+        <v>44861.510416666664</v>
+      </c>
+      <c r="B6102" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6102" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6103">
+      <c r="A6103" s="6" t="n">
+        <v>44861.520833333336</v>
+      </c>
+      <c r="B6103" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6103" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6104">
+      <c r="A6104" s="6" t="n">
+        <v>44861.53125</v>
+      </c>
+      <c r="B6104" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6104" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6105">
+      <c r="A6105" s="6" t="n">
+        <v>44861.541666666664</v>
+      </c>
+      <c r="B6105" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6105" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6106">
+      <c r="A6106" s="6" t="n">
+        <v>44861.552083333336</v>
+      </c>
+      <c r="B6106" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6106" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6107">
+      <c r="A6107" s="6" t="n">
+        <v>44861.5625</v>
+      </c>
+      <c r="B6107" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6107" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6108">
+      <c r="A6108" s="6" t="n">
+        <v>44861.572916666664</v>
+      </c>
+      <c r="B6108" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6108" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6109">
+      <c r="A6109" s="6" t="n">
+        <v>44861.583333333336</v>
+      </c>
+      <c r="B6109" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6109" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6110">
+      <c r="A6110" s="6" t="n">
+        <v>44861.59375</v>
+      </c>
+      <c r="B6110" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6110" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6111">
+      <c r="A6111" s="6" t="n">
+        <v>44861.604166666664</v>
+      </c>
+      <c r="B6111" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6111" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6112">
+      <c r="A6112" s="6" t="n">
+        <v>44861.614583333336</v>
+      </c>
+      <c r="B6112" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6112" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6113">
+      <c r="A6113" s="6" t="n">
+        <v>44861.625</v>
+      </c>
+      <c r="B6113" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6113" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6114">
+      <c r="A6114" s="6" t="n">
+        <v>44861.635416666664</v>
+      </c>
+      <c r="B6114" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6114" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6115">
+      <c r="A6115" s="6" t="n">
+        <v>44861.645833333336</v>
+      </c>
+      <c r="B6115" s="1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C6115" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6116">
+      <c r="A6116" s="6" t="n">
+        <v>44861.65625</v>
+      </c>
+      <c r="B6116" s="1" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="C6116" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6117">
+      <c r="A6117" s="6" t="n">
+        <v>44861.666666666664</v>
+      </c>
+      <c r="B6117" s="1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C6117" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6118">
+      <c r="A6118" s="6" t="n">
+        <v>44861.677083333336</v>
+      </c>
+      <c r="B6118" s="1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C6118" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6119">
+      <c r="A6119" s="6" t="n">
+        <v>44861.6875</v>
+      </c>
+      <c r="B6119" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C6119" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6120">
+      <c r="A6120" s="6" t="n">
+        <v>44861.697916666664</v>
+      </c>
+      <c r="B6120" s="1" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="C6120" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6121">
+      <c r="A6121" s="6" t="n">
+        <v>44861.708333333336</v>
+      </c>
+      <c r="B6121" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C6121" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6122">
+      <c r="A6122" s="6" t="n">
+        <v>44861.71875</v>
+      </c>
+      <c r="B6122" s="1" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C6122" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6123">
+      <c r="A6123" s="6" t="n">
+        <v>44861.729166666664</v>
+      </c>
+      <c r="B6123" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6123" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="6124">
+      <c r="A6124" s="6" t="n">
+        <v>44861.739583333336</v>
+      </c>
+      <c r="B6124" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6124" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6125">
+      <c r="A6125" s="6" t="n">
+        <v>44861.75</v>
+      </c>
+      <c r="B6125" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6125" s="1" t="n">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="6126">
+      <c r="A6126" s="6" t="n">
+        <v>44861.760416666664</v>
+      </c>
+      <c r="B6126" s="1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C6126" s="1" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="6127">
+      <c r="A6127" s="6" t="n">
+        <v>44861.770833333336</v>
+      </c>
+      <c r="B6127" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6127" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6128">
+      <c r="A6128" s="6" t="n">
+        <v>44861.78125</v>
+      </c>
+      <c r="B6128" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6128" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="6129">
+      <c r="A6129" s="6" t="n">
+        <v>44861.791666666664</v>
+      </c>
+      <c r="B6129" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6129" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6130">
+      <c r="A6130" s="6" t="n">
+        <v>44861.802083333336</v>
+      </c>
+      <c r="B6130" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6130" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6131">
+      <c r="A6131" s="6" t="n">
+        <v>44861.8125</v>
+      </c>
+      <c r="B6131" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6131" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6132">
+      <c r="A6132" s="6" t="n">
+        <v>44861.822916666664</v>
+      </c>
+      <c r="B6132" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6132" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6133">
+      <c r="A6133" s="6" t="n">
+        <v>44861.833333333336</v>
+      </c>
+      <c r="B6133" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6133" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6134">
+      <c r="A6134" s="6" t="n">
+        <v>44861.84375</v>
+      </c>
+      <c r="B6134" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6134" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6135">
+      <c r="A6135" s="6" t="n">
+        <v>44861.854166666664</v>
+      </c>
+      <c r="B6135" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6135" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6136">
+      <c r="A6136" s="6" t="n">
+        <v>44861.864583333336</v>
+      </c>
+      <c r="B6136" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6136" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6137">
+      <c r="A6137" s="6" t="n">
+        <v>44861.875</v>
+      </c>
+      <c r="B6137" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6137" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6138">
+      <c r="A6138" s="6" t="n">
+        <v>44861.885416666664</v>
+      </c>
+      <c r="B6138" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6138" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6139">
+      <c r="A6139" s="6" t="n">
+        <v>44861.895833333336</v>
+      </c>
+      <c r="B6139" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6139" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6140">
+      <c r="A6140" s="6" t="n">
+        <v>44861.90625</v>
+      </c>
+      <c r="B6140" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6140" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6141">
+      <c r="A6141" s="6" t="n">
+        <v>44861.916666666664</v>
+      </c>
+      <c r="B6141" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6141" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6142">
+      <c r="A6142" s="6" t="n">
+        <v>44861.927083333336</v>
+      </c>
+      <c r="B6142" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6142" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6143">
+      <c r="A6143" s="6" t="n">
+        <v>44861.9375</v>
+      </c>
+      <c r="B6143" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6143" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6144">
+      <c r="A6144" s="6" t="n">
+        <v>44861.947916666664</v>
+      </c>
+      <c r="B6144" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6144" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6145">
+      <c r="A6145" s="6" t="n">
+        <v>44861.958333333336</v>
+      </c>
+      <c r="B6145" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6145" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6146">
+      <c r="A6146" s="6" t="n">
+        <v>44861.96875</v>
+      </c>
+      <c r="B6146" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6146" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6147">
+      <c r="A6147" s="6" t="n">
+        <v>44861.979166666664</v>
+      </c>
+      <c r="B6147" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6147" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6148">
+      <c r="A6148" s="6" t="n">
+        <v>44861.989583333336</v>
+      </c>
+      <c r="B6148" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6148" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6149">
+      <c r="A6149" s="6" t="n">
+        <v>44862.0</v>
+      </c>
+      <c r="B6149" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6149" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6150">
+      <c r="A6150" s="6" t="n">
+        <v>44862.010416666664</v>
+      </c>
+      <c r="B6150" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6150" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6151">
+      <c r="A6151" s="6" t="n">
+        <v>44862.020833333336</v>
+      </c>
+      <c r="B6151" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6151" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6152">
+      <c r="A6152" s="6" t="n">
+        <v>44862.03125</v>
+      </c>
+      <c r="B6152" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6152" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6153">
+      <c r="A6153" s="6" t="n">
+        <v>44862.041666666664</v>
+      </c>
+      <c r="B6153" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6153" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6154">
+      <c r="A6154" s="6" t="n">
+        <v>44862.052083333336</v>
+      </c>
+      <c r="B6154" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6154" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6155">
+      <c r="A6155" s="6" t="n">
+        <v>44862.0625</v>
+      </c>
+      <c r="B6155" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6155" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6156">
+      <c r="A6156" s="6" t="n">
+        <v>44862.072916666664</v>
+      </c>
+      <c r="B6156" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6156" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6157">
+      <c r="A6157" s="6" t="n">
+        <v>44862.083333333336</v>
+      </c>
+      <c r="B6157" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6157" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6158">
+      <c r="A6158" s="6" t="n">
+        <v>44862.09375</v>
+      </c>
+      <c r="B6158" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6158" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6159">
+      <c r="A6159" s="6" t="n">
+        <v>44862.104166666664</v>
+      </c>
+      <c r="B6159" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6159" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6160">
+      <c r="A6160" s="6" t="n">
+        <v>44862.114583333336</v>
+      </c>
+      <c r="B6160" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6160" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6161">
+      <c r="A6161" s="6" t="n">
+        <v>44862.125</v>
+      </c>
+      <c r="B6161" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6161" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6162">
+      <c r="A6162" s="6" t="n">
+        <v>44862.135416666664</v>
+      </c>
+      <c r="B6162" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6162" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6163">
+      <c r="A6163" s="6" t="n">
+        <v>44862.145833333336</v>
+      </c>
+      <c r="B6163" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6163" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6164">
+      <c r="A6164" s="6" t="n">
+        <v>44862.15625</v>
+      </c>
+      <c r="B6164" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6164" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6165">
+      <c r="A6165" s="6" t="n">
+        <v>44862.166666666664</v>
+      </c>
+      <c r="B6165" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6165" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6166">
+      <c r="A6166" s="6" t="n">
+        <v>44862.177083333336</v>
+      </c>
+      <c r="B6166" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6166" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6167">
+      <c r="A6167" s="6" t="n">
+        <v>44862.1875</v>
+      </c>
+      <c r="B6167" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6167" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6168">
+      <c r="A6168" s="6" t="n">
+        <v>44862.197916666664</v>
+      </c>
+      <c r="B6168" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6168" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6169">
+      <c r="A6169" s="6" t="n">
+        <v>44862.208333333336</v>
+      </c>
+      <c r="B6169" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6169" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6170">
+      <c r="A6170" s="6" t="n">
+        <v>44862.21875</v>
+      </c>
+      <c r="B6170" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6170" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6171">
+      <c r="A6171" s="6" t="n">
+        <v>44862.229166666664</v>
+      </c>
+      <c r="B6171" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6171" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6172">
+      <c r="A6172" s="6" t="n">
+        <v>44862.239583333336</v>
+      </c>
+      <c r="B6172" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6172" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6173">
+      <c r="A6173" s="6" t="n">
+        <v>44862.25</v>
+      </c>
+      <c r="B6173" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6173" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6174">
+      <c r="A6174" s="6" t="n">
+        <v>44862.260416666664</v>
+      </c>
+      <c r="B6174" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6174" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6175">
+      <c r="A6175" s="6" t="n">
+        <v>44862.270833333336</v>
+      </c>
+      <c r="B6175" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6175" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6176">
+      <c r="A6176" s="6" t="n">
+        <v>44862.28125</v>
+      </c>
+      <c r="B6176" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6176" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6177">
+      <c r="A6177" s="6" t="n">
+        <v>44862.291666666664</v>
+      </c>
+      <c r="B6177" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6177" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6178">
+      <c r="A6178" s="6" t="n">
+        <v>44862.302083333336</v>
+      </c>
+      <c r="B6178" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6178" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6179">
+      <c r="A6179" s="6" t="n">
+        <v>44862.3125</v>
+      </c>
+      <c r="B6179" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6179" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6180">
+      <c r="A6180" s="6" t="n">
+        <v>44862.322916666664</v>
+      </c>
+      <c r="B6180" s="1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C6180" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6181">
+      <c r="A6181" s="6" t="n">
+        <v>44862.333333333336</v>
+      </c>
+      <c r="B6181" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6181" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6182">
+      <c r="A6182" s="6" t="n">
+        <v>44862.34375</v>
+      </c>
+      <c r="B6182" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6182" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6183">
+      <c r="A6183" s="6" t="n">
+        <v>44862.354166666664</v>
+      </c>
+      <c r="B6183" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6183" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6184">
+      <c r="A6184" s="6" t="n">
+        <v>44862.364583333336</v>
+      </c>
+      <c r="B6184" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6184" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6185">
+      <c r="A6185" s="6" t="n">
+        <v>44862.375</v>
+      </c>
+      <c r="B6185" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6185" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6186">
+      <c r="A6186" s="6" t="n">
+        <v>44862.385416666664</v>
+      </c>
+      <c r="B6186" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6186" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="6187">
+      <c r="A6187" s="6" t="n">
+        <v>44862.395833333336</v>
+      </c>
+      <c r="B6187" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6187" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6188">
+      <c r="A6188" s="6" t="n">
+        <v>44862.40625</v>
+      </c>
+      <c r="B6188" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6188" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6189">
+      <c r="A6189" s="6" t="n">
+        <v>44862.416666666664</v>
+      </c>
+      <c r="B6189" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6189" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6190">
+      <c r="A6190" s="6" t="n">
+        <v>44862.427083333336</v>
+      </c>
+      <c r="B6190" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6190" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6191">
+      <c r="A6191" s="6" t="n">
+        <v>44862.4375</v>
+      </c>
+      <c r="B6191" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6191" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6192">
+      <c r="A6192" s="6" t="n">
+        <v>44862.447916666664</v>
+      </c>
+      <c r="B6192" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6192" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6193">
+      <c r="A6193" s="6" t="n">
+        <v>44862.458333333336</v>
+      </c>
+      <c r="B6193" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6193" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6194">
+      <c r="A6194" s="6" t="n">
+        <v>44862.46875</v>
+      </c>
+      <c r="B6194" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6194" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6195">
+      <c r="A6195" s="6" t="n">
+        <v>44862.479166666664</v>
+      </c>
+      <c r="B6195" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6195" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6196">
+      <c r="A6196" s="6" t="n">
+        <v>44862.489583333336</v>
+      </c>
+      <c r="B6196" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6196" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6197">
+      <c r="A6197" s="6" t="n">
+        <v>44862.5</v>
+      </c>
+      <c r="B6197" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6197" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6198">
+      <c r="A6198" s="6" t="n">
+        <v>44862.510416666664</v>
+      </c>
+      <c r="B6198" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6198" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6199">
+      <c r="A6199" s="6" t="n">
+        <v>44862.520833333336</v>
+      </c>
+      <c r="B6199" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6199" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6200">
+      <c r="A6200" s="6" t="n">
+        <v>44862.53125</v>
+      </c>
+      <c r="B6200" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6200" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6201">
+      <c r="A6201" s="6" t="n">
+        <v>44862.541666666664</v>
+      </c>
+      <c r="B6201" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6201" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6202">
+      <c r="A6202" s="6" t="n">
+        <v>44862.552083333336</v>
+      </c>
+      <c r="B6202" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6202" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6203">
+      <c r="A6203" s="6" t="n">
+        <v>44862.5625</v>
+      </c>
+      <c r="B6203" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6203" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6204">
+      <c r="A6204" s="6" t="n">
+        <v>44862.572916666664</v>
+      </c>
+      <c r="B6204" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6204" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="6205">
+      <c r="A6205" s="6" t="n">
+        <v>44862.583333333336</v>
+      </c>
+      <c r="B6205" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C6205" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6206">
+      <c r="A6206" s="6" t="n">
+        <v>44862.59375</v>
+      </c>
+      <c r="B6206" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6206" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6207">
+      <c r="A6207" s="6" t="n">
+        <v>44862.604166666664</v>
+      </c>
+      <c r="B6207" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6207" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6208">
+      <c r="A6208" s="6" t="n">
+        <v>44862.614583333336</v>
+      </c>
+      <c r="B6208" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6208" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6209">
+      <c r="A6209" s="6" t="n">
+        <v>44862.625</v>
+      </c>
+      <c r="B6209" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6209" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6210">
+      <c r="A6210" s="6" t="n">
+        <v>44862.635416666664</v>
+      </c>
+      <c r="B6210" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C6210" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6211">
+      <c r="A6211" s="6" t="n">
+        <v>44862.645833333336</v>
+      </c>
+      <c r="B6211" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6211" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6212">
+      <c r="A6212" s="6" t="n">
+        <v>44862.65625</v>
+      </c>
+      <c r="B6212" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6212" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6213">
+      <c r="A6213" s="6" t="n">
+        <v>44862.666666666664</v>
+      </c>
+      <c r="B6213" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6213" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6214">
+      <c r="A6214" s="6" t="n">
+        <v>44862.677083333336</v>
+      </c>
+      <c r="B6214" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C6214" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6215">
+      <c r="A6215" s="6" t="n">
+        <v>44862.6875</v>
+      </c>
+      <c r="B6215" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6215" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6216">
+      <c r="A6216" s="6" t="n">
+        <v>44862.697916666664</v>
+      </c>
+      <c r="B6216" s="1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C6216" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6217">
+      <c r="A6217" s="6" t="n">
+        <v>44862.708333333336</v>
+      </c>
+      <c r="B6217" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C6217" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6218">
+      <c r="A6218" s="6" t="n">
+        <v>44862.71875</v>
+      </c>
+      <c r="B6218" s="1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C6218" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6219">
+      <c r="A6219" s="6" t="n">
+        <v>44862.729166666664</v>
+      </c>
+      <c r="B6219" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6219" s="1" t="n">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="6220">
+      <c r="A6220" s="6" t="n">
+        <v>44862.739583333336</v>
+      </c>
+      <c r="B6220" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6220" s="1" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="6221">
+      <c r="A6221" s="6" t="n">
+        <v>44862.75</v>
+      </c>
+      <c r="B6221" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6221" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6222">
+      <c r="A6222" s="6" t="n">
+        <v>44862.760416666664</v>
+      </c>
+      <c r="B6222" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6222" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6223">
+      <c r="A6223" s="6" t="n">
+        <v>44862.770833333336</v>
+      </c>
+      <c r="B6223" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6223" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6224">
+      <c r="A6224" s="6" t="n">
+        <v>44862.78125</v>
+      </c>
+      <c r="B6224" s="1" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="C6224" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6225">
+      <c r="A6225" s="6" t="n">
+        <v>44862.791666666664</v>
+      </c>
+      <c r="B6225" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6225" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6226">
+      <c r="A6226" s="6" t="n">
+        <v>44862.802083333336</v>
+      </c>
+      <c r="B6226" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6226" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6227">
+      <c r="A6227" s="6" t="n">
+        <v>44862.8125</v>
+      </c>
+      <c r="B6227" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6227" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6228">
+      <c r="A6228" s="6" t="n">
+        <v>44862.822916666664</v>
+      </c>
+      <c r="B6228" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6228" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6229">
+      <c r="A6229" s="6" t="n">
+        <v>44862.833333333336</v>
+      </c>
+      <c r="B6229" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6229" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6230">
+      <c r="A6230" s="6" t="n">
+        <v>44862.84375</v>
+      </c>
+      <c r="B6230" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6230" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6231">
+      <c r="A6231" s="6" t="n">
+        <v>44862.854166666664</v>
+      </c>
+      <c r="B6231" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6231" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6232">
+      <c r="A6232" s="6" t="n">
+        <v>44862.864583333336</v>
+      </c>
+      <c r="B6232" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6232" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6233">
+      <c r="A6233" s="6" t="n">
+        <v>44862.875</v>
+      </c>
+      <c r="B6233" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6233" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6234">
+      <c r="A6234" s="6" t="n">
+        <v>44862.885416666664</v>
+      </c>
+      <c r="B6234" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6234" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6235">
+      <c r="A6235" s="6" t="n">
+        <v>44862.895833333336</v>
+      </c>
+      <c r="B6235" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6235" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6236">
+      <c r="A6236" s="6" t="n">
+        <v>44862.90625</v>
+      </c>
+      <c r="B6236" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6236" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6237">
+      <c r="A6237" s="6" t="n">
+        <v>44862.916666666664</v>
+      </c>
+      <c r="B6237" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6237" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6238">
+      <c r="A6238" s="6" t="n">
+        <v>44862.927083333336</v>
+      </c>
+      <c r="B6238" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6238" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6239">
+      <c r="A6239" s="6" t="n">
+        <v>44862.9375</v>
+      </c>
+      <c r="B6239" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C6239" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6240">
+      <c r="A6240" s="6" t="n">
+        <v>44862.947916666664</v>
+      </c>
+      <c r="B6240" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6240" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6241">
+      <c r="A6241" s="6" t="n">
+        <v>44862.958333333336</v>
+      </c>
+      <c r="B6241" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6241" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6242">
+      <c r="A6242" s="6" t="n">
+        <v>44862.96875</v>
+      </c>
+      <c r="B6242" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6242" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6243">
+      <c r="A6243" s="6" t="n">
+        <v>44862.979166666664</v>
+      </c>
+      <c r="B6243" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6243" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6244">
+      <c r="A6244" s="6" t="n">
+        <v>44862.989583333336</v>
+      </c>
+      <c r="B6244" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6244" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6245">
+      <c r="A6245" s="6" t="n">
+        <v>44863.0</v>
+      </c>
+      <c r="B6245" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6245" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6246">
+      <c r="A6246" s="6" t="n">
+        <v>44863.010416666664</v>
+      </c>
+      <c r="B6246" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6246" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6247">
+      <c r="A6247" s="6" t="n">
+        <v>44863.020833333336</v>
+      </c>
+      <c r="B6247" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6247" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6248">
+      <c r="A6248" s="6" t="n">
+        <v>44863.03125</v>
+      </c>
+      <c r="B6248" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6248" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6249">
+      <c r="A6249" s="6" t="n">
+        <v>44863.041666666664</v>
+      </c>
+      <c r="B6249" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6249" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6250">
+      <c r="A6250" s="6" t="n">
+        <v>44863.052083333336</v>
+      </c>
+      <c r="B6250" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6250" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6251">
+      <c r="A6251" s="6" t="n">
+        <v>44863.0625</v>
+      </c>
+      <c r="B6251" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6251" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6252">
+      <c r="A6252" s="6" t="n">
+        <v>44863.072916666664</v>
+      </c>
+      <c r="B6252" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6252" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6253">
+      <c r="A6253" s="6" t="n">
+        <v>44863.083333333336</v>
+      </c>
+      <c r="B6253" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6253" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6254">
+      <c r="A6254" s="6" t="n">
+        <v>44863.09375</v>
+      </c>
+      <c r="B6254" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6254" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6255">
+      <c r="A6255" s="6" t="n">
+        <v>44863.104166666664</v>
+      </c>
+      <c r="B6255" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6255" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6256">
+      <c r="A6256" s="6" t="n">
+        <v>44863.114583333336</v>
+      </c>
+      <c r="B6256" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6256" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6257">
+      <c r="A6257" s="6" t="n">
+        <v>44863.125</v>
+      </c>
+      <c r="B6257" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6257" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6258">
+      <c r="A6258" s="6" t="n">
+        <v>44863.135416666664</v>
+      </c>
+      <c r="B6258" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6258" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6259">
+      <c r="A6259" s="6" t="n">
+        <v>44863.145833333336</v>
+      </c>
+      <c r="B6259" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6259" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6260">
+      <c r="A6260" s="6" t="n">
+        <v>44863.15625</v>
+      </c>
+      <c r="B6260" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6260" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6261">
+      <c r="A6261" s="6" t="n">
+        <v>44863.166666666664</v>
+      </c>
+      <c r="B6261" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6261" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6262">
+      <c r="A6262" s="6" t="n">
+        <v>44863.177083333336</v>
+      </c>
+      <c r="B6262" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6262" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6263">
+      <c r="A6263" s="6" t="n">
+        <v>44863.1875</v>
+      </c>
+      <c r="B6263" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6263" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6264">
+      <c r="A6264" s="6" t="n">
+        <v>44863.197916666664</v>
+      </c>
+      <c r="B6264" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6264" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6265">
+      <c r="A6265" s="6" t="n">
+        <v>44863.208333333336</v>
+      </c>
+      <c r="B6265" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6265" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6266">
+      <c r="A6266" s="6" t="n">
+        <v>44863.21875</v>
+      </c>
+      <c r="B6266" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6266" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6267">
+      <c r="A6267" s="6" t="n">
+        <v>44863.229166666664</v>
+      </c>
+      <c r="B6267" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6267" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6268">
+      <c r="A6268" s="6" t="n">
+        <v>44863.239583333336</v>
+      </c>
+      <c r="B6268" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6268" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6269">
+      <c r="A6269" s="6" t="n">
+        <v>44863.25</v>
+      </c>
+      <c r="B6269" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6269" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6270">
+      <c r="A6270" s="6" t="n">
+        <v>44863.260416666664</v>
+      </c>
+      <c r="B6270" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6270" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6271">
+      <c r="A6271" s="6" t="n">
+        <v>44863.270833333336</v>
+      </c>
+      <c r="B6271" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6271" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6272">
+      <c r="A6272" s="6" t="n">
+        <v>44863.28125</v>
+      </c>
+      <c r="B6272" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6272" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6273">
+      <c r="A6273" s="6" t="n">
+        <v>44863.291666666664</v>
+      </c>
+      <c r="B6273" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6273" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6274">
+      <c r="A6274" s="6" t="n">
+        <v>44863.302083333336</v>
+      </c>
+      <c r="B6274" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6274" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6275">
+      <c r="A6275" s="6" t="n">
+        <v>44863.3125</v>
+      </c>
+      <c r="B6275" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6275" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6276">
+      <c r="A6276" s="6" t="n">
+        <v>44863.322916666664</v>
+      </c>
+      <c r="B6276" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6276" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6277">
+      <c r="A6277" s="6" t="n">
+        <v>44863.333333333336</v>
+      </c>
+      <c r="B6277" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6277" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6278">
+      <c r="A6278" s="6" t="n">
+        <v>44863.34375</v>
+      </c>
+      <c r="B6278" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6278" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6279">
+      <c r="A6279" s="6" t="n">
+        <v>44863.354166666664</v>
+      </c>
+      <c r="B6279" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6279" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6280">
+      <c r="A6280" s="6" t="n">
+        <v>44863.364583333336</v>
+      </c>
+      <c r="B6280" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6280" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6281">
+      <c r="A6281" s="6" t="n">
+        <v>44863.375</v>
+      </c>
+      <c r="B6281" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6281" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6282">
+      <c r="A6282" s="6" t="n">
+        <v>44863.385416666664</v>
+      </c>
+      <c r="B6282" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6282" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6283">
+      <c r="A6283" s="6" t="n">
+        <v>44863.395833333336</v>
+      </c>
+      <c r="B6283" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6283" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6284">
+      <c r="A6284" s="6" t="n">
+        <v>44863.40625</v>
+      </c>
+      <c r="B6284" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6284" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6285">
+      <c r="A6285" s="6" t="n">
+        <v>44863.416666666664</v>
+      </c>
+      <c r="B6285" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6285" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6286">
+      <c r="A6286" s="6" t="n">
+        <v>44863.427083333336</v>
+      </c>
+      <c r="B6286" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6286" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="6287">
+      <c r="A6287" s="6" t="n">
+        <v>44863.4375</v>
+      </c>
+      <c r="B6287" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6287" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6288">
+      <c r="A6288" s="6" t="n">
+        <v>44863.447916666664</v>
+      </c>
+      <c r="B6288" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6288" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6289">
+      <c r="A6289" s="6" t="n">
+        <v>44863.458333333336</v>
+      </c>
+      <c r="B6289" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6289" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6290">
+      <c r="A6290" s="6" t="n">
+        <v>44863.46875</v>
+      </c>
+      <c r="B6290" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6290" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6291">
+      <c r="A6291" s="6" t="n">
+        <v>44863.479166666664</v>
+      </c>
+      <c r="B6291" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6291" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6292">
+      <c r="A6292" s="6" t="n">
+        <v>44863.489583333336</v>
+      </c>
+      <c r="B6292" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6292" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6293">
+      <c r="A6293" s="6" t="n">
+        <v>44863.5</v>
+      </c>
+      <c r="B6293" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6293" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6294">
+      <c r="A6294" s="6" t="n">
+        <v>44863.510416666664</v>
+      </c>
+      <c r="B6294" s="1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C6294" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6295">
+      <c r="A6295" s="6" t="n">
+        <v>44863.520833333336</v>
+      </c>
+      <c r="B6295" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6295" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6296">
+      <c r="A6296" s="6" t="n">
+        <v>44863.53125</v>
+      </c>
+      <c r="B6296" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6296" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6297">
+      <c r="A6297" s="6" t="n">
+        <v>44863.541666666664</v>
+      </c>
+      <c r="B6297" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6297" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6298">
+      <c r="A6298" s="6" t="n">
+        <v>44863.552083333336</v>
+      </c>
+      <c r="B6298" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6298" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6299">
+      <c r="A6299" s="6" t="n">
+        <v>44863.5625</v>
+      </c>
+      <c r="B6299" s="1"/>
+      <c r="C6299" s="1"/>
+    </row>
+    <row r="6300">
+      <c r="A6300" s="6" t="n">
+        <v>44863.572916666664</v>
+      </c>
+      <c r="B6300" s="1"/>
+      <c r="C6300" s="1"/>
+    </row>
+    <row r="6301">
+      <c r="A6301" s="6" t="n">
+        <v>44863.583333333336</v>
+      </c>
+      <c r="B6301" s="1"/>
+      <c r="C6301" s="1"/>
+    </row>
+    <row r="6302">
+      <c r="A6302" s="6" t="n">
+        <v>44863.59375</v>
+      </c>
+      <c r="B6302" s="1"/>
+      <c r="C6302" s="1"/>
+    </row>
+    <row r="6303">
+      <c r="A6303" s="6" t="n">
+        <v>44863.604166666664</v>
+      </c>
+      <c r="B6303" s="1"/>
+      <c r="C6303" s="1"/>
+    </row>
+    <row r="6304">
+      <c r="A6304" s="6" t="n">
+        <v>44863.614583333336</v>
+      </c>
+      <c r="B6304" s="1"/>
+      <c r="C6304" s="1"/>
+    </row>
+    <row r="6305">
+      <c r="A6305" s="6" t="n">
+        <v>44863.625</v>
+      </c>
+      <c r="B6305" s="1"/>
+      <c r="C6305" s="1"/>
+    </row>
+    <row r="6306">
+      <c r="A6306" s="6" t="n">
+        <v>44863.635416666664</v>
+      </c>
+      <c r="B6306" s="1"/>
+      <c r="C6306" s="1"/>
+    </row>
+    <row r="6307">
+      <c r="A6307" s="6" t="n">
+        <v>44863.645833333336</v>
+      </c>
+      <c r="B6307" s="1"/>
+      <c r="C6307" s="1"/>
+    </row>
+    <row r="6308">
+      <c r="A6308" s="6" t="n">
+        <v>44863.65625</v>
+      </c>
+      <c r="B6308" s="1"/>
+      <c r="C6308" s="1"/>
+    </row>
+    <row r="6309">
+      <c r="A6309" s="6" t="n">
+        <v>44863.666666666664</v>
+      </c>
+      <c r="B6309" s="1"/>
+      <c r="C6309" s="1"/>
+    </row>
+    <row r="6310">
+      <c r="A6310" s="6" t="n">
+        <v>44863.677083333336</v>
+      </c>
+      <c r="B6310" s="1"/>
+      <c r="C6310" s="1"/>
+    </row>
+    <row r="6311">
+      <c r="A6311" s="6" t="n">
+        <v>44863.6875</v>
+      </c>
+      <c r="B6311" s="1"/>
+      <c r="C6311" s="1"/>
+    </row>
+    <row r="6312">
+      <c r="A6312" s="6" t="n">
+        <v>44863.697916666664</v>
+      </c>
+      <c r="B6312" s="1"/>
+      <c r="C6312" s="1"/>
+    </row>
+    <row r="6313">
+      <c r="A6313" s="6" t="n">
+        <v>44863.708333333336</v>
+      </c>
+      <c r="B6313" s="1"/>
+      <c r="C6313" s="1"/>
+    </row>
+    <row r="6314">
+      <c r="A6314" s="6" t="n">
+        <v>44863.71875</v>
+      </c>
+      <c r="B6314" s="1"/>
+      <c r="C6314" s="1"/>
+    </row>
+    <row r="6315">
+      <c r="A6315" s="6" t="n">
+        <v>44863.729166666664</v>
+      </c>
+      <c r="B6315" s="1"/>
+      <c r="C6315" s="1"/>
+    </row>
+    <row r="6316">
+      <c r="A6316" s="6" t="n">
+        <v>44863.739583333336</v>
+      </c>
+      <c r="B6316" s="1"/>
+      <c r="C6316" s="1"/>
+    </row>
+    <row r="6317">
+      <c r="A6317" s="6" t="n">
+        <v>44863.75</v>
+      </c>
+      <c r="B6317" s="1"/>
+      <c r="C6317" s="1"/>
+    </row>
+    <row r="6318">
+      <c r="A6318" s="6" t="n">
+        <v>44863.760416666664</v>
+      </c>
+      <c r="B6318" s="1"/>
+      <c r="C6318" s="1"/>
+    </row>
+    <row r="6319">
+      <c r="A6319" s="6" t="n">
+        <v>44863.770833333336</v>
+      </c>
+      <c r="B6319" s="1"/>
+      <c r="C6319" s="1"/>
+    </row>
+    <row r="6320">
+      <c r="A6320" s="6" t="n">
+        <v>44863.78125</v>
+      </c>
+      <c r="B6320" s="1"/>
+      <c r="C6320" s="1"/>
+    </row>
+    <row r="6321">
+      <c r="A6321" s="6" t="n">
+        <v>44863.791666666664</v>
+      </c>
+      <c r="B6321" s="1"/>
+      <c r="C6321" s="1"/>
+    </row>
+    <row r="6322">
+      <c r="A6322" s="6" t="n">
+        <v>44863.802083333336</v>
+      </c>
+      <c r="B6322" s="1"/>
+      <c r="C6322" s="1"/>
+    </row>
+    <row r="6323">
+      <c r="A6323" s="6" t="n">
+        <v>44863.8125</v>
+      </c>
+      <c r="B6323" s="1"/>
+      <c r="C6323" s="1"/>
+    </row>
+    <row r="6324">
+      <c r="A6324" s="6" t="n">
+        <v>44863.822916666664</v>
+      </c>
+      <c r="B6324" s="1"/>
+      <c r="C6324" s="1"/>
+    </row>
+    <row r="6325">
+      <c r="A6325" s="6" t="n">
+        <v>44863.833333333336</v>
+      </c>
+      <c r="B6325" s="1"/>
+      <c r="C6325" s="1"/>
+    </row>
+    <row r="6326">
+      <c r="A6326" s="6" t="n">
+        <v>44863.84375</v>
+      </c>
+      <c r="B6326" s="1"/>
+      <c r="C6326" s="1"/>
+    </row>
+    <row r="6327">
+      <c r="A6327" s="6" t="n">
+        <v>44863.854166666664</v>
+      </c>
+      <c r="B6327" s="1"/>
+      <c r="C6327" s="1"/>
+    </row>
+    <row r="6328">
+      <c r="A6328" s="6" t="n">
+        <v>44863.864583333336</v>
+      </c>
+      <c r="B6328" s="1"/>
+      <c r="C6328" s="1"/>
+    </row>
+    <row r="6329">
+      <c r="A6329" s="6" t="n">
+        <v>44863.875</v>
+      </c>
+      <c r="B6329" s="1"/>
+      <c r="C6329" s="1"/>
+    </row>
+    <row r="6330">
+      <c r="A6330" s="6" t="n">
+        <v>44863.885416666664</v>
+      </c>
+      <c r="B6330" s="1"/>
+      <c r="C6330" s="1"/>
+    </row>
+    <row r="6331">
+      <c r="A6331" s="6" t="n">
+        <v>44863.895833333336</v>
+      </c>
+      <c r="B6331" s="1"/>
+      <c r="C6331" s="1"/>
+    </row>
+    <row r="6332">
+      <c r="A6332" s="6" t="n">
+        <v>44863.90625</v>
+      </c>
+      <c r="B6332" s="1"/>
+      <c r="C6332" s="1"/>
+    </row>
+    <row r="6333">
+      <c r="A6333" s="6" t="n">
+        <v>44863.916666666664</v>
+      </c>
+      <c r="B6333" s="1"/>
+      <c r="C6333" s="1"/>
+    </row>
+    <row r="6334">
+      <c r="A6334" s="6" t="n">
+        <v>44863.927083333336</v>
+      </c>
+      <c r="B6334" s="1"/>
+      <c r="C6334" s="1"/>
+    </row>
+    <row r="6335">
+      <c r="A6335" s="6" t="n">
+        <v>44863.9375</v>
+      </c>
+      <c r="B6335" s="1"/>
+      <c r="C6335" s="1"/>
+    </row>
+    <row r="6336">
+      <c r="A6336" s="6" t="n">
+        <v>44863.947916666664</v>
+      </c>
+      <c r="B6336" s="1"/>
+      <c r="C6336" s="1"/>
+    </row>
+    <row r="6337">
+      <c r="A6337" s="6" t="n">
+        <v>44863.958333333336</v>
+      </c>
+      <c r="B6337" s="1"/>
+      <c r="C6337" s="1"/>
+    </row>
+    <row r="6338">
+      <c r="A6338" s="6" t="n">
+        <v>44863.96875</v>
+      </c>
+      <c r="B6338" s="1"/>
+      <c r="C6338" s="1"/>
+    </row>
+    <row r="6339">
+      <c r="A6339" s="6" t="n">
+        <v>44863.979166666664</v>
+      </c>
+      <c r="B6339" s="1"/>
+      <c r="C6339" s="1"/>
+    </row>
+    <row r="6340">
+      <c r="A6340" s="6" t="n">
+        <v>44863.989583333336</v>
+      </c>
+      <c r="B6340" s="1"/>
+      <c r="C6340" s="1"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>